<commit_message>
Aggiunte alcune misurazioni bf2 su GTX1070
</commit_message>
<xml_diff>
--- a/performance bf2.xlsx
+++ b/performance bf2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Filippo\Desktop\tesi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE4ECE83-A8E7-46CD-A969-042B563574BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B8EF593-4E89-4799-A58B-B5188342FFF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="24">
   <si>
     <t>SPEEDUP</t>
   </si>
@@ -91,6 +91,9 @@
   </si>
   <si>
     <t>RTX 2080</t>
+  </si>
+  <si>
+    <t>THROUGHPUT</t>
   </si>
   <si>
     <t>bf2-aos-nosh</t>
@@ -596,10 +599,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:T89"/>
+  <dimension ref="A1:AO83"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F54" sqref="F54"/>
+      <selection activeCell="AD9" sqref="AD9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -609,19 +612,28 @@
     <col min="3" max="20" width="8.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A1" s="20" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="20"/>
       <c r="C1" s="20"/>
-    </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="V1" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="W1" s="20"/>
+      <c r="X1" s="20"/>
+    </row>
+    <row r="2" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A2" s="20"/>
       <c r="B2" s="20"/>
       <c r="C2" s="20"/>
-    </row>
-    <row r="3" spans="1:20" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="U2" s="15"/>
+      <c r="V2" s="20"/>
+      <c r="W2" s="20"/>
+      <c r="X2" s="20"/>
+    </row>
+    <row r="3" spans="1:41" ht="18.75" x14ac:dyDescent="0.25">
       <c r="C3" s="21" t="s">
         <v>16</v>
       </c>
@@ -646,8 +658,35 @@
       <c r="R3" s="21"/>
       <c r="S3" s="21"/>
       <c r="T3" s="21"/>
-    </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U3" s="15"/>
+      <c r="V3" s="17"/>
+      <c r="W3" s="1"/>
+      <c r="X3" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="Y3" s="21"/>
+      <c r="Z3" s="21"/>
+      <c r="AA3" s="21"/>
+      <c r="AB3" s="21"/>
+      <c r="AC3" s="21"/>
+      <c r="AD3" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="AE3" s="21"/>
+      <c r="AF3" s="21"/>
+      <c r="AG3" s="21"/>
+      <c r="AH3" s="21"/>
+      <c r="AI3" s="21"/>
+      <c r="AJ3" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="AK3" s="21"/>
+      <c r="AL3" s="21"/>
+      <c r="AM3" s="21"/>
+      <c r="AN3" s="21"/>
+      <c r="AO3" s="21"/>
+    </row>
+    <row r="4" spans="1:41" x14ac:dyDescent="0.25">
       <c r="C4" s="2" t="s">
         <v>10</v>
       </c>
@@ -702,10 +741,67 @@
       <c r="T4" s="3" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U4" s="15"/>
+      <c r="V4" s="17"/>
+      <c r="W4" s="1"/>
+      <c r="X4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="Y4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="Z4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="AA4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="AB4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="AC4" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="AD4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="AE4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="AF4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="AG4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="AH4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="AI4" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="AJ4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="AK4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="AL4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="AM4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="AN4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="AO4" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:41" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="19" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>1</v>
@@ -737,8 +833,42 @@
         <f>AVERAGE(O5:S5)</f>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U5" s="15"/>
+      <c r="V5" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="W5" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="X5" s="6"/>
+      <c r="Y5" s="7"/>
+      <c r="Z5" s="7"/>
+      <c r="AA5" s="7"/>
+      <c r="AB5" s="8"/>
+      <c r="AC5" s="5" t="e">
+        <f>AVERAGE(X5:AB5)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AD5" s="6"/>
+      <c r="AE5" s="7"/>
+      <c r="AF5" s="7"/>
+      <c r="AG5" s="7"/>
+      <c r="AH5" s="8"/>
+      <c r="AI5" s="5" t="e">
+        <f>AVERAGE(AD5:AH5)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AJ5" s="6"/>
+      <c r="AK5" s="7"/>
+      <c r="AL5" s="7"/>
+      <c r="AM5" s="7"/>
+      <c r="AN5" s="8"/>
+      <c r="AO5" s="5" t="e">
+        <f>AVERAGE(AJ5:AN5)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="6" spans="1:41" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="19"/>
       <c r="B6" s="4" t="s">
         <v>2</v>
@@ -752,14 +882,16 @@
         <f t="shared" ref="H6:H13" si="0">AVERAGE(C6:G6)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="I6" s="9"/>
+      <c r="I6" s="9">
+        <v>118.693</v>
+      </c>
       <c r="J6" s="10"/>
       <c r="K6" s="10"/>
       <c r="L6" s="10"/>
       <c r="M6" s="11"/>
-      <c r="N6" s="5" t="e">
+      <c r="N6" s="5">
         <f t="shared" ref="N6:N13" si="1">AVERAGE(I6:M6)</f>
-        <v>#DIV/0!</v>
+        <v>118.693</v>
       </c>
       <c r="O6" s="9"/>
       <c r="P6" s="10"/>
@@ -770,8 +902,42 @@
         <f t="shared" ref="T6:T13" si="2">AVERAGE(O6:S6)</f>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U6" s="15"/>
+      <c r="V6" s="19"/>
+      <c r="W6" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="X6" s="9"/>
+      <c r="Y6" s="10"/>
+      <c r="Z6" s="10"/>
+      <c r="AA6" s="10"/>
+      <c r="AB6" s="10"/>
+      <c r="AC6" s="5" t="e">
+        <f t="shared" ref="AC6:AC13" si="3">AVERAGE(X6:AB6)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AD6" s="9">
+        <v>49.54</v>
+      </c>
+      <c r="AE6" s="10"/>
+      <c r="AF6" s="10"/>
+      <c r="AG6" s="10"/>
+      <c r="AH6" s="11"/>
+      <c r="AI6" s="5">
+        <f t="shared" ref="AI6:AI13" si="4">AVERAGE(AD6:AH6)</f>
+        <v>49.54</v>
+      </c>
+      <c r="AJ6" s="9"/>
+      <c r="AK6" s="10"/>
+      <c r="AL6" s="10"/>
+      <c r="AM6" s="10"/>
+      <c r="AN6" s="11"/>
+      <c r="AO6" s="5" t="e">
+        <f t="shared" ref="AO6:AO13" si="5">AVERAGE(AJ6:AN6)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="7" spans="1:41" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="19"/>
       <c r="B7" s="4" t="s">
         <v>3</v>
@@ -785,14 +951,16 @@
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="I7" s="9"/>
+      <c r="I7" s="9">
+        <v>464.947</v>
+      </c>
       <c r="J7" s="10"/>
       <c r="K7" s="10"/>
       <c r="L7" s="10"/>
       <c r="M7" s="11"/>
-      <c r="N7" s="5" t="e">
+      <c r="N7" s="5">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+        <v>464.947</v>
       </c>
       <c r="O7" s="9"/>
       <c r="P7" s="10"/>
@@ -803,8 +971,42 @@
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U7" s="15"/>
+      <c r="V7" s="19"/>
+      <c r="W7" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="X7" s="9"/>
+      <c r="Y7" s="10"/>
+      <c r="Z7" s="10"/>
+      <c r="AA7" s="10"/>
+      <c r="AB7" s="10"/>
+      <c r="AC7" s="5" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AD7" s="9">
+        <v>44.88</v>
+      </c>
+      <c r="AE7" s="10"/>
+      <c r="AF7" s="10"/>
+      <c r="AG7" s="10"/>
+      <c r="AH7" s="10"/>
+      <c r="AI7" s="5">
+        <f t="shared" si="4"/>
+        <v>44.88</v>
+      </c>
+      <c r="AJ7" s="9"/>
+      <c r="AK7" s="10"/>
+      <c r="AL7" s="10"/>
+      <c r="AM7" s="10"/>
+      <c r="AN7" s="11"/>
+      <c r="AO7" s="5" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="8" spans="1:41" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="19"/>
       <c r="B8" s="4" t="s">
         <v>4</v>
@@ -818,14 +1020,16 @@
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="I8" s="9"/>
+      <c r="I8" s="9">
+        <v>1822.7090000000001</v>
+      </c>
       <c r="J8" s="10"/>
       <c r="K8" s="10"/>
       <c r="L8" s="10"/>
       <c r="M8" s="11"/>
-      <c r="N8" s="5" t="e">
+      <c r="N8" s="5">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+        <v>1822.7090000000001</v>
       </c>
       <c r="O8" s="9"/>
       <c r="P8" s="10"/>
@@ -836,8 +1040,42 @@
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U8" s="15"/>
+      <c r="V8" s="19"/>
+      <c r="W8" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="X8" s="9"/>
+      <c r="Y8" s="10"/>
+      <c r="Z8" s="10"/>
+      <c r="AA8" s="10"/>
+      <c r="AB8" s="10"/>
+      <c r="AC8" s="5" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AD8" s="9">
+        <v>45.43</v>
+      </c>
+      <c r="AE8" s="10"/>
+      <c r="AF8" s="10"/>
+      <c r="AG8" s="10"/>
+      <c r="AH8" s="10"/>
+      <c r="AI8" s="5">
+        <f t="shared" si="4"/>
+        <v>45.43</v>
+      </c>
+      <c r="AJ8" s="9"/>
+      <c r="AK8" s="10"/>
+      <c r="AL8" s="10"/>
+      <c r="AM8" s="10"/>
+      <c r="AN8" s="11"/>
+      <c r="AO8" s="5" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="9" spans="1:41" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="19"/>
       <c r="B9" s="4" t="s">
         <v>5</v>
@@ -869,8 +1107,40 @@
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U9" s="15"/>
+      <c r="V9" s="19"/>
+      <c r="W9" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="X9" s="9"/>
+      <c r="Y9" s="10"/>
+      <c r="Z9" s="10"/>
+      <c r="AA9" s="10"/>
+      <c r="AB9" s="10"/>
+      <c r="AC9" s="5" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AD9" s="9"/>
+      <c r="AE9" s="10"/>
+      <c r="AF9" s="10"/>
+      <c r="AG9" s="10"/>
+      <c r="AH9" s="10"/>
+      <c r="AI9" s="5" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AJ9" s="9"/>
+      <c r="AK9" s="10"/>
+      <c r="AL9" s="10"/>
+      <c r="AM9" s="10"/>
+      <c r="AN9" s="11"/>
+      <c r="AO9" s="5" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="10" spans="1:41" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="19"/>
       <c r="B10" s="4" t="s">
         <v>6</v>
@@ -902,8 +1172,40 @@
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U10" s="15"/>
+      <c r="V10" s="19"/>
+      <c r="W10" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="X10" s="9"/>
+      <c r="Y10" s="10"/>
+      <c r="Z10" s="10"/>
+      <c r="AA10" s="10"/>
+      <c r="AB10" s="11"/>
+      <c r="AC10" s="5" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AD10" s="9"/>
+      <c r="AE10" s="10"/>
+      <c r="AF10" s="10"/>
+      <c r="AG10" s="10"/>
+      <c r="AH10" s="11"/>
+      <c r="AI10" s="5" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AJ10" s="9"/>
+      <c r="AK10" s="10"/>
+      <c r="AL10" s="10"/>
+      <c r="AM10" s="10"/>
+      <c r="AN10" s="11"/>
+      <c r="AO10" s="5" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="11" spans="1:41" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="19"/>
       <c r="B11" s="4" t="s">
         <v>7</v>
@@ -935,8 +1237,40 @@
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U11" s="15"/>
+      <c r="V11" s="19"/>
+      <c r="W11" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="X11" s="9"/>
+      <c r="Y11" s="10"/>
+      <c r="Z11" s="10"/>
+      <c r="AA11" s="10"/>
+      <c r="AB11" s="11"/>
+      <c r="AC11" s="5" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AD11" s="9"/>
+      <c r="AE11" s="10"/>
+      <c r="AF11" s="10"/>
+      <c r="AG11" s="10"/>
+      <c r="AH11" s="11"/>
+      <c r="AI11" s="5" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AJ11" s="9"/>
+      <c r="AK11" s="10"/>
+      <c r="AL11" s="10"/>
+      <c r="AM11" s="10"/>
+      <c r="AN11" s="11"/>
+      <c r="AO11" s="5" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="12" spans="1:41" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="19"/>
       <c r="B12" s="4" t="s">
         <v>8</v>
@@ -968,8 +1302,40 @@
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U12" s="15"/>
+      <c r="V12" s="19"/>
+      <c r="W12" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="X12" s="9"/>
+      <c r="Y12" s="10"/>
+      <c r="Z12" s="10"/>
+      <c r="AA12" s="10"/>
+      <c r="AB12" s="11"/>
+      <c r="AC12" s="5" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AD12" s="9"/>
+      <c r="AE12" s="10"/>
+      <c r="AF12" s="10"/>
+      <c r="AG12" s="10"/>
+      <c r="AH12" s="11"/>
+      <c r="AI12" s="5" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AJ12" s="9"/>
+      <c r="AK12" s="10"/>
+      <c r="AL12" s="10"/>
+      <c r="AM12" s="10"/>
+      <c r="AN12" s="11"/>
+      <c r="AO12" s="5" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="13" spans="1:41" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="19"/>
       <c r="B13" s="4" t="s">
         <v>9</v>
@@ -1001,8 +1367,40 @@
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U13" s="15"/>
+      <c r="V13" s="19"/>
+      <c r="W13" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="X13" s="12"/>
+      <c r="Y13" s="13"/>
+      <c r="Z13" s="13"/>
+      <c r="AA13" s="13"/>
+      <c r="AB13" s="14"/>
+      <c r="AC13" s="5" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AD13" s="12"/>
+      <c r="AE13" s="13"/>
+      <c r="AF13" s="13"/>
+      <c r="AG13" s="13"/>
+      <c r="AH13" s="14"/>
+      <c r="AI13" s="5" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AJ13" s="12"/>
+      <c r="AK13" s="13"/>
+      <c r="AL13" s="13"/>
+      <c r="AM13" s="13"/>
+      <c r="AN13" s="14"/>
+      <c r="AO13" s="5" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="14" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A14" s="18"/>
       <c r="B14" s="16"/>
       <c r="C14" s="15"/>
@@ -1023,10 +1421,31 @@
       <c r="R14" s="15"/>
       <c r="S14" s="15"/>
       <c r="T14" s="15"/>
-    </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U14" s="15"/>
+      <c r="V14" s="18"/>
+      <c r="W14" s="16"/>
+      <c r="X14" s="15"/>
+      <c r="Y14" s="15"/>
+      <c r="Z14" s="15"/>
+      <c r="AA14" s="15"/>
+      <c r="AB14" s="15"/>
+      <c r="AC14" s="15"/>
+      <c r="AD14" s="15"/>
+      <c r="AE14" s="15"/>
+      <c r="AF14" s="15"/>
+      <c r="AG14" s="15"/>
+      <c r="AH14" s="15"/>
+      <c r="AI14" s="15"/>
+      <c r="AJ14" s="15"/>
+      <c r="AK14" s="15"/>
+      <c r="AL14" s="15"/>
+      <c r="AM14" s="15"/>
+      <c r="AN14" s="15"/>
+      <c r="AO14" s="15"/>
+    </row>
+    <row r="15" spans="1:41" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="19" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B15" s="4" t="s">
         <v>1</v>
@@ -1058,8 +1477,42 @@
         <f>AVERAGE(O15:S15)</f>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U15" s="15"/>
+      <c r="V15" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="W15" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="X15" s="6"/>
+      <c r="Y15" s="7"/>
+      <c r="Z15" s="7"/>
+      <c r="AA15" s="7"/>
+      <c r="AB15" s="8"/>
+      <c r="AC15" s="5" t="e">
+        <f>AVERAGE(X15:AB15)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AD15" s="6"/>
+      <c r="AE15" s="7"/>
+      <c r="AF15" s="7"/>
+      <c r="AG15" s="7"/>
+      <c r="AH15" s="8"/>
+      <c r="AI15" s="5" t="e">
+        <f>AVERAGE(AD15:AH15)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AJ15" s="6"/>
+      <c r="AK15" s="7"/>
+      <c r="AL15" s="7"/>
+      <c r="AM15" s="7"/>
+      <c r="AN15" s="8"/>
+      <c r="AO15" s="5" t="e">
+        <f>AVERAGE(AJ15:AN15)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="16" spans="1:41" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="19"/>
       <c r="B16" s="4" t="s">
         <v>2</v>
@@ -1070,7 +1523,7 @@
       <c r="F16" s="10"/>
       <c r="G16" s="11"/>
       <c r="H16" s="5" t="e">
-        <f t="shared" ref="H16:H23" si="3">AVERAGE(C16:G16)</f>
+        <f t="shared" ref="H16:H23" si="6">AVERAGE(C16:G16)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="I16" s="9"/>
@@ -1079,7 +1532,7 @@
       <c r="L16" s="10"/>
       <c r="M16" s="11"/>
       <c r="N16" s="5" t="e">
-        <f t="shared" ref="N16:N23" si="4">AVERAGE(I16:M16)</f>
+        <f t="shared" ref="N16:N23" si="7">AVERAGE(I16:M16)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="O16" s="9"/>
@@ -1088,11 +1541,43 @@
       <c r="R16" s="10"/>
       <c r="S16" s="11"/>
       <c r="T16" s="5" t="e">
-        <f t="shared" ref="T16:T23" si="5">AVERAGE(O16:S16)</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
+        <f t="shared" ref="T16:T23" si="8">AVERAGE(O16:S16)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="U16" s="15"/>
+      <c r="V16" s="19"/>
+      <c r="W16" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="X16" s="9"/>
+      <c r="Y16" s="10"/>
+      <c r="Z16" s="10"/>
+      <c r="AA16" s="10"/>
+      <c r="AB16" s="11"/>
+      <c r="AC16" s="5" t="e">
+        <f t="shared" ref="AC16:AC23" si="9">AVERAGE(X16:AB16)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AD16" s="9"/>
+      <c r="AE16" s="10"/>
+      <c r="AF16" s="10"/>
+      <c r="AG16" s="10"/>
+      <c r="AH16" s="11"/>
+      <c r="AI16" s="5" t="e">
+        <f t="shared" ref="AI16:AI23" si="10">AVERAGE(AD16:AH16)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AJ16" s="9"/>
+      <c r="AK16" s="10"/>
+      <c r="AL16" s="10"/>
+      <c r="AM16" s="10"/>
+      <c r="AN16" s="11"/>
+      <c r="AO16" s="5" t="e">
+        <f t="shared" ref="AO16:AO23" si="11">AVERAGE(AJ16:AN16)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="17" spans="1:41" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="19"/>
       <c r="B17" s="4" t="s">
         <v>3</v>
@@ -1103,7 +1588,7 @@
       <c r="F17" s="10"/>
       <c r="G17" s="11"/>
       <c r="H17" s="5" t="e">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I17" s="9"/>
@@ -1112,7 +1597,7 @@
       <c r="L17" s="10"/>
       <c r="M17" s="11"/>
       <c r="N17" s="5" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>#DIV/0!</v>
       </c>
       <c r="O17" s="9"/>
@@ -1121,11 +1606,43 @@
       <c r="R17" s="10"/>
       <c r="S17" s="11"/>
       <c r="T17" s="5" t="e">
-        <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
+        <f t="shared" si="8"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="U17" s="15"/>
+      <c r="V17" s="19"/>
+      <c r="W17" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="X17" s="9"/>
+      <c r="Y17" s="10"/>
+      <c r="Z17" s="10"/>
+      <c r="AA17" s="10"/>
+      <c r="AB17" s="10"/>
+      <c r="AC17" s="5" t="e">
+        <f t="shared" si="9"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AD17" s="9"/>
+      <c r="AE17" s="10"/>
+      <c r="AF17" s="10"/>
+      <c r="AG17" s="10"/>
+      <c r="AH17" s="10"/>
+      <c r="AI17" s="5" t="e">
+        <f t="shared" si="10"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AJ17" s="9"/>
+      <c r="AK17" s="10"/>
+      <c r="AL17" s="10"/>
+      <c r="AM17" s="10"/>
+      <c r="AN17" s="11"/>
+      <c r="AO17" s="5" t="e">
+        <f t="shared" si="11"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="18" spans="1:41" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="19"/>
       <c r="B18" s="4" t="s">
         <v>4</v>
@@ -1136,7 +1653,7 @@
       <c r="F18" s="10"/>
       <c r="G18" s="11"/>
       <c r="H18" s="5" t="e">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I18" s="9"/>
@@ -1145,7 +1662,7 @@
       <c r="L18" s="10"/>
       <c r="M18" s="11"/>
       <c r="N18" s="5" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>#DIV/0!</v>
       </c>
       <c r="O18" s="9"/>
@@ -1154,11 +1671,43 @@
       <c r="R18" s="10"/>
       <c r="S18" s="11"/>
       <c r="T18" s="5" t="e">
-        <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
+        <f t="shared" si="8"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="U18" s="15"/>
+      <c r="V18" s="19"/>
+      <c r="W18" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="X18" s="9"/>
+      <c r="Y18" s="10"/>
+      <c r="Z18" s="10"/>
+      <c r="AA18" s="10"/>
+      <c r="AB18" s="10"/>
+      <c r="AC18" s="5" t="e">
+        <f t="shared" si="9"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AD18" s="9"/>
+      <c r="AE18" s="10"/>
+      <c r="AF18" s="10"/>
+      <c r="AG18" s="10"/>
+      <c r="AH18" s="10"/>
+      <c r="AI18" s="5" t="e">
+        <f t="shared" si="10"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AJ18" s="9"/>
+      <c r="AK18" s="10"/>
+      <c r="AL18" s="10"/>
+      <c r="AM18" s="10"/>
+      <c r="AN18" s="11"/>
+      <c r="AO18" s="5" t="e">
+        <f t="shared" si="11"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="19" spans="1:41" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="19"/>
       <c r="B19" s="4" t="s">
         <v>5</v>
@@ -1169,7 +1718,7 @@
       <c r="F19" s="10"/>
       <c r="G19" s="11"/>
       <c r="H19" s="5" t="e">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I19" s="9"/>
@@ -1178,7 +1727,7 @@
       <c r="L19" s="10"/>
       <c r="M19" s="11"/>
       <c r="N19" s="5" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>#DIV/0!</v>
       </c>
       <c r="O19" s="9"/>
@@ -1187,11 +1736,43 @@
       <c r="R19" s="10"/>
       <c r="S19" s="11"/>
       <c r="T19" s="5" t="e">
-        <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
+        <f t="shared" si="8"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="U19" s="15"/>
+      <c r="V19" s="19"/>
+      <c r="W19" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="X19" s="9"/>
+      <c r="Y19" s="10"/>
+      <c r="Z19" s="10"/>
+      <c r="AA19" s="10"/>
+      <c r="AB19" s="10"/>
+      <c r="AC19" s="5" t="e">
+        <f t="shared" si="9"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AD19" s="9"/>
+      <c r="AE19" s="10"/>
+      <c r="AF19" s="10"/>
+      <c r="AG19" s="10"/>
+      <c r="AH19" s="10"/>
+      <c r="AI19" s="5" t="e">
+        <f t="shared" si="10"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AJ19" s="9"/>
+      <c r="AK19" s="10"/>
+      <c r="AL19" s="10"/>
+      <c r="AM19" s="10"/>
+      <c r="AN19" s="11"/>
+      <c r="AO19" s="5" t="e">
+        <f t="shared" si="11"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="20" spans="1:41" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="19"/>
       <c r="B20" s="4" t="s">
         <v>6</v>
@@ -1202,7 +1783,7 @@
       <c r="F20" s="10"/>
       <c r="G20" s="11"/>
       <c r="H20" s="5" t="e">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I20" s="9"/>
@@ -1211,7 +1792,7 @@
       <c r="L20" s="10"/>
       <c r="M20" s="11"/>
       <c r="N20" s="5" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>#DIV/0!</v>
       </c>
       <c r="O20" s="9"/>
@@ -1220,11 +1801,43 @@
       <c r="R20" s="10"/>
       <c r="S20" s="11"/>
       <c r="T20" s="5" t="e">
-        <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
+        <f t="shared" si="8"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="U20" s="15"/>
+      <c r="V20" s="19"/>
+      <c r="W20" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="X20" s="9"/>
+      <c r="Y20" s="10"/>
+      <c r="Z20" s="10"/>
+      <c r="AA20" s="10"/>
+      <c r="AB20" s="11"/>
+      <c r="AC20" s="5" t="e">
+        <f t="shared" si="9"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AD20" s="9"/>
+      <c r="AE20" s="10"/>
+      <c r="AF20" s="10"/>
+      <c r="AG20" s="10"/>
+      <c r="AH20" s="11"/>
+      <c r="AI20" s="5" t="e">
+        <f t="shared" si="10"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AJ20" s="9"/>
+      <c r="AK20" s="10"/>
+      <c r="AL20" s="10"/>
+      <c r="AM20" s="10"/>
+      <c r="AN20" s="11"/>
+      <c r="AO20" s="5" t="e">
+        <f t="shared" si="11"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="21" spans="1:41" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="19"/>
       <c r="B21" s="4" t="s">
         <v>7</v>
@@ -1235,7 +1848,7 @@
       <c r="F21" s="10"/>
       <c r="G21" s="11"/>
       <c r="H21" s="5" t="e">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I21" s="9"/>
@@ -1244,7 +1857,7 @@
       <c r="L21" s="10"/>
       <c r="M21" s="11"/>
       <c r="N21" s="5" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>#DIV/0!</v>
       </c>
       <c r="O21" s="9"/>
@@ -1253,11 +1866,43 @@
       <c r="R21" s="10"/>
       <c r="S21" s="11"/>
       <c r="T21" s="5" t="e">
-        <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
+        <f t="shared" si="8"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="U21" s="15"/>
+      <c r="V21" s="19"/>
+      <c r="W21" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="X21" s="9"/>
+      <c r="Y21" s="10"/>
+      <c r="Z21" s="10"/>
+      <c r="AA21" s="10"/>
+      <c r="AB21" s="11"/>
+      <c r="AC21" s="5" t="e">
+        <f t="shared" si="9"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AD21" s="9"/>
+      <c r="AE21" s="10"/>
+      <c r="AF21" s="10"/>
+      <c r="AG21" s="10"/>
+      <c r="AH21" s="11"/>
+      <c r="AI21" s="5" t="e">
+        <f t="shared" si="10"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AJ21" s="9"/>
+      <c r="AK21" s="10"/>
+      <c r="AL21" s="10"/>
+      <c r="AM21" s="10"/>
+      <c r="AN21" s="11"/>
+      <c r="AO21" s="5" t="e">
+        <f t="shared" si="11"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="22" spans="1:41" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="19"/>
       <c r="B22" s="4" t="s">
         <v>8</v>
@@ -1268,7 +1913,7 @@
       <c r="F22" s="10"/>
       <c r="G22" s="11"/>
       <c r="H22" s="5" t="e">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I22" s="9"/>
@@ -1277,7 +1922,7 @@
       <c r="L22" s="10"/>
       <c r="M22" s="11"/>
       <c r="N22" s="5" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>#DIV/0!</v>
       </c>
       <c r="O22" s="9"/>
@@ -1286,11 +1931,43 @@
       <c r="R22" s="10"/>
       <c r="S22" s="11"/>
       <c r="T22" s="5" t="e">
-        <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
+        <f t="shared" si="8"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="U22" s="15"/>
+      <c r="V22" s="19"/>
+      <c r="W22" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="X22" s="9"/>
+      <c r="Y22" s="10"/>
+      <c r="Z22" s="10"/>
+      <c r="AA22" s="10"/>
+      <c r="AB22" s="11"/>
+      <c r="AC22" s="5" t="e">
+        <f t="shared" si="9"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AD22" s="9"/>
+      <c r="AE22" s="10"/>
+      <c r="AF22" s="10"/>
+      <c r="AG22" s="10"/>
+      <c r="AH22" s="11"/>
+      <c r="AI22" s="5" t="e">
+        <f t="shared" si="10"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AJ22" s="9"/>
+      <c r="AK22" s="10"/>
+      <c r="AL22" s="10"/>
+      <c r="AM22" s="10"/>
+      <c r="AN22" s="11"/>
+      <c r="AO22" s="5" t="e">
+        <f t="shared" si="11"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="23" spans="1:41" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="19"/>
       <c r="B23" s="4" t="s">
         <v>9</v>
@@ -1301,7 +1978,7 @@
       <c r="F23" s="13"/>
       <c r="G23" s="14"/>
       <c r="H23" s="5" t="e">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I23" s="12"/>
@@ -1310,7 +1987,7 @@
       <c r="L23" s="13"/>
       <c r="M23" s="14"/>
       <c r="N23" s="5" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>#DIV/0!</v>
       </c>
       <c r="O23" s="12"/>
@@ -1319,11 +1996,43 @@
       <c r="R23" s="13"/>
       <c r="S23" s="14"/>
       <c r="T23" s="5" t="e">
-        <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
+        <f t="shared" si="8"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="U23" s="15"/>
+      <c r="V23" s="19"/>
+      <c r="W23" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="X23" s="12"/>
+      <c r="Y23" s="13"/>
+      <c r="Z23" s="13"/>
+      <c r="AA23" s="13"/>
+      <c r="AB23" s="14"/>
+      <c r="AC23" s="5" t="e">
+        <f t="shared" si="9"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AD23" s="12"/>
+      <c r="AE23" s="13"/>
+      <c r="AF23" s="13"/>
+      <c r="AG23" s="13"/>
+      <c r="AH23" s="14"/>
+      <c r="AI23" s="5" t="e">
+        <f t="shared" si="10"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AJ23" s="12"/>
+      <c r="AK23" s="13"/>
+      <c r="AL23" s="13"/>
+      <c r="AM23" s="13"/>
+      <c r="AN23" s="14"/>
+      <c r="AO23" s="5" t="e">
+        <f t="shared" si="11"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="24" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A24" s="18"/>
       <c r="B24" s="16"/>
       <c r="C24" s="15"/>
@@ -1344,10 +2053,31 @@
       <c r="R24" s="15"/>
       <c r="S24" s="15"/>
       <c r="T24" s="15"/>
-    </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U24" s="15"/>
+      <c r="V24" s="18"/>
+      <c r="W24" s="16"/>
+      <c r="X24" s="15"/>
+      <c r="Y24" s="15"/>
+      <c r="Z24" s="15"/>
+      <c r="AA24" s="15"/>
+      <c r="AB24" s="15"/>
+      <c r="AC24" s="15"/>
+      <c r="AD24" s="15"/>
+      <c r="AE24" s="15"/>
+      <c r="AF24" s="15"/>
+      <c r="AG24" s="15"/>
+      <c r="AH24" s="15"/>
+      <c r="AI24" s="15"/>
+      <c r="AJ24" s="15"/>
+      <c r="AK24" s="15"/>
+      <c r="AL24" s="15"/>
+      <c r="AM24" s="15"/>
+      <c r="AN24" s="15"/>
+      <c r="AO24" s="15"/>
+    </row>
+    <row r="25" spans="1:41" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="19" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B25" s="4" t="s">
         <v>1</v>
@@ -1379,8 +2109,42 @@
         <f>AVERAGE(O25:S25)</f>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U25" s="15"/>
+      <c r="V25" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="W25" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="X25" s="6"/>
+      <c r="Y25" s="7"/>
+      <c r="Z25" s="7"/>
+      <c r="AA25" s="7"/>
+      <c r="AB25" s="8"/>
+      <c r="AC25" s="5" t="e">
+        <f>AVERAGE(X25:AB25)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AD25" s="6"/>
+      <c r="AE25" s="7"/>
+      <c r="AF25" s="7"/>
+      <c r="AG25" s="7"/>
+      <c r="AH25" s="8"/>
+      <c r="AI25" s="5" t="e">
+        <f>AVERAGE(AD25:AH25)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AJ25" s="6"/>
+      <c r="AK25" s="7"/>
+      <c r="AL25" s="7"/>
+      <c r="AM25" s="7"/>
+      <c r="AN25" s="8"/>
+      <c r="AO25" s="5" t="e">
+        <f>AVERAGE(AJ25:AN25)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="26" spans="1:41" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="19"/>
       <c r="B26" s="4" t="s">
         <v>2</v>
@@ -1391,7 +2155,7 @@
       <c r="F26" s="10"/>
       <c r="G26" s="11"/>
       <c r="H26" s="5" t="e">
-        <f t="shared" ref="H26:H33" si="6">AVERAGE(C26:G26)</f>
+        <f t="shared" ref="H26:H33" si="12">AVERAGE(C26:G26)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="I26" s="9"/>
@@ -1400,7 +2164,7 @@
       <c r="L26" s="10"/>
       <c r="M26" s="11"/>
       <c r="N26" s="5" t="e">
-        <f t="shared" ref="N26:N33" si="7">AVERAGE(I26:M26)</f>
+        <f t="shared" ref="N26:N33" si="13">AVERAGE(I26:M26)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="O26" s="9"/>
@@ -1409,11 +2173,43 @@
       <c r="R26" s="10"/>
       <c r="S26" s="11"/>
       <c r="T26" s="5" t="e">
-        <f t="shared" ref="T26:T33" si="8">AVERAGE(O26:S26)</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
+        <f t="shared" ref="T26:T33" si="14">AVERAGE(O26:S26)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="U26" s="15"/>
+      <c r="V26" s="19"/>
+      <c r="W26" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="X26" s="9"/>
+      <c r="Y26" s="10"/>
+      <c r="Z26" s="10"/>
+      <c r="AA26" s="10"/>
+      <c r="AB26" s="11"/>
+      <c r="AC26" s="5" t="e">
+        <f t="shared" ref="AC26:AC33" si="15">AVERAGE(X26:AB26)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AD26" s="9"/>
+      <c r="AE26" s="10"/>
+      <c r="AF26" s="10"/>
+      <c r="AG26" s="10"/>
+      <c r="AH26" s="11"/>
+      <c r="AI26" s="5" t="e">
+        <f t="shared" ref="AI26:AI33" si="16">AVERAGE(AD26:AH26)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AJ26" s="9"/>
+      <c r="AK26" s="10"/>
+      <c r="AL26" s="10"/>
+      <c r="AM26" s="10"/>
+      <c r="AN26" s="11"/>
+      <c r="AO26" s="5" t="e">
+        <f t="shared" ref="AO26:AO33" si="17">AVERAGE(AJ26:AN26)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="27" spans="1:41" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="19"/>
       <c r="B27" s="4" t="s">
         <v>3</v>
@@ -1424,7 +2220,7 @@
       <c r="F27" s="10"/>
       <c r="G27" s="11"/>
       <c r="H27" s="5" t="e">
-        <f t="shared" si="6"/>
+        <f t="shared" si="12"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I27" s="9"/>
@@ -1433,7 +2229,7 @@
       <c r="L27" s="10"/>
       <c r="M27" s="11"/>
       <c r="N27" s="5" t="e">
-        <f t="shared" si="7"/>
+        <f t="shared" si="13"/>
         <v>#DIV/0!</v>
       </c>
       <c r="O27" s="9"/>
@@ -1442,11 +2238,43 @@
       <c r="R27" s="10"/>
       <c r="S27" s="11"/>
       <c r="T27" s="5" t="e">
-        <f t="shared" si="8"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
+        <f t="shared" si="14"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="U27" s="15"/>
+      <c r="V27" s="19"/>
+      <c r="W27" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="X27" s="9"/>
+      <c r="Y27" s="10"/>
+      <c r="Z27" s="10"/>
+      <c r="AA27" s="10"/>
+      <c r="AB27" s="10"/>
+      <c r="AC27" s="5" t="e">
+        <f t="shared" si="15"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AD27" s="9"/>
+      <c r="AE27" s="10"/>
+      <c r="AF27" s="10"/>
+      <c r="AG27" s="10"/>
+      <c r="AH27" s="10"/>
+      <c r="AI27" s="5" t="e">
+        <f t="shared" si="16"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AJ27" s="9"/>
+      <c r="AK27" s="10"/>
+      <c r="AL27" s="10"/>
+      <c r="AM27" s="10"/>
+      <c r="AN27" s="11"/>
+      <c r="AO27" s="5" t="e">
+        <f t="shared" si="17"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="28" spans="1:41" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="19"/>
       <c r="B28" s="4" t="s">
         <v>4</v>
@@ -1457,7 +2285,7 @@
       <c r="F28" s="10"/>
       <c r="G28" s="11"/>
       <c r="H28" s="5" t="e">
-        <f t="shared" si="6"/>
+        <f t="shared" si="12"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I28" s="9"/>
@@ -1466,7 +2294,7 @@
       <c r="L28" s="10"/>
       <c r="M28" s="11"/>
       <c r="N28" s="5" t="e">
-        <f t="shared" si="7"/>
+        <f t="shared" si="13"/>
         <v>#DIV/0!</v>
       </c>
       <c r="O28" s="9"/>
@@ -1475,11 +2303,43 @@
       <c r="R28" s="10"/>
       <c r="S28" s="11"/>
       <c r="T28" s="5" t="e">
-        <f t="shared" si="8"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
+        <f t="shared" si="14"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="U28" s="15"/>
+      <c r="V28" s="19"/>
+      <c r="W28" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="X28" s="9"/>
+      <c r="Y28" s="10"/>
+      <c r="Z28" s="10"/>
+      <c r="AA28" s="10"/>
+      <c r="AB28" s="10"/>
+      <c r="AC28" s="5" t="e">
+        <f t="shared" si="15"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AD28" s="9"/>
+      <c r="AE28" s="10"/>
+      <c r="AF28" s="10"/>
+      <c r="AG28" s="10"/>
+      <c r="AH28" s="10"/>
+      <c r="AI28" s="5" t="e">
+        <f t="shared" si="16"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AJ28" s="9"/>
+      <c r="AK28" s="10"/>
+      <c r="AL28" s="10"/>
+      <c r="AM28" s="10"/>
+      <c r="AN28" s="11"/>
+      <c r="AO28" s="5" t="e">
+        <f t="shared" si="17"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="29" spans="1:41" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="19"/>
       <c r="B29" s="4" t="s">
         <v>5</v>
@@ -1490,7 +2350,7 @@
       <c r="F29" s="10"/>
       <c r="G29" s="11"/>
       <c r="H29" s="5" t="e">
-        <f t="shared" si="6"/>
+        <f t="shared" si="12"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I29" s="9"/>
@@ -1499,7 +2359,7 @@
       <c r="L29" s="10"/>
       <c r="M29" s="11"/>
       <c r="N29" s="5" t="e">
-        <f t="shared" si="7"/>
+        <f t="shared" si="13"/>
         <v>#DIV/0!</v>
       </c>
       <c r="O29" s="9"/>
@@ -1508,11 +2368,43 @@
       <c r="R29" s="10"/>
       <c r="S29" s="11"/>
       <c r="T29" s="5" t="e">
-        <f t="shared" si="8"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
+        <f t="shared" si="14"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="U29" s="15"/>
+      <c r="V29" s="19"/>
+      <c r="W29" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="X29" s="9"/>
+      <c r="Y29" s="10"/>
+      <c r="Z29" s="10"/>
+      <c r="AA29" s="10"/>
+      <c r="AB29" s="10"/>
+      <c r="AC29" s="5" t="e">
+        <f t="shared" si="15"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AD29" s="9"/>
+      <c r="AE29" s="10"/>
+      <c r="AF29" s="10"/>
+      <c r="AG29" s="10"/>
+      <c r="AH29" s="10"/>
+      <c r="AI29" s="5" t="e">
+        <f t="shared" si="16"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AJ29" s="9"/>
+      <c r="AK29" s="10"/>
+      <c r="AL29" s="10"/>
+      <c r="AM29" s="10"/>
+      <c r="AN29" s="11"/>
+      <c r="AO29" s="5" t="e">
+        <f t="shared" si="17"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="30" spans="1:41" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="19"/>
       <c r="B30" s="4" t="s">
         <v>6</v>
@@ -1523,7 +2415,7 @@
       <c r="F30" s="10"/>
       <c r="G30" s="11"/>
       <c r="H30" s="5" t="e">
-        <f t="shared" si="6"/>
+        <f t="shared" si="12"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I30" s="9"/>
@@ -1532,7 +2424,7 @@
       <c r="L30" s="10"/>
       <c r="M30" s="11"/>
       <c r="N30" s="5" t="e">
-        <f t="shared" si="7"/>
+        <f t="shared" si="13"/>
         <v>#DIV/0!</v>
       </c>
       <c r="O30" s="9"/>
@@ -1541,11 +2433,43 @@
       <c r="R30" s="10"/>
       <c r="S30" s="11"/>
       <c r="T30" s="5" t="e">
-        <f t="shared" si="8"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
+        <f t="shared" si="14"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="U30" s="15"/>
+      <c r="V30" s="19"/>
+      <c r="W30" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="X30" s="9"/>
+      <c r="Y30" s="10"/>
+      <c r="Z30" s="10"/>
+      <c r="AA30" s="10"/>
+      <c r="AB30" s="11"/>
+      <c r="AC30" s="5" t="e">
+        <f t="shared" si="15"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AD30" s="9"/>
+      <c r="AE30" s="10"/>
+      <c r="AF30" s="10"/>
+      <c r="AG30" s="10"/>
+      <c r="AH30" s="11"/>
+      <c r="AI30" s="5" t="e">
+        <f t="shared" si="16"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AJ30" s="9"/>
+      <c r="AK30" s="10"/>
+      <c r="AL30" s="10"/>
+      <c r="AM30" s="10"/>
+      <c r="AN30" s="11"/>
+      <c r="AO30" s="5" t="e">
+        <f t="shared" si="17"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="31" spans="1:41" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="19"/>
       <c r="B31" s="4" t="s">
         <v>7</v>
@@ -1556,7 +2480,7 @@
       <c r="F31" s="10"/>
       <c r="G31" s="11"/>
       <c r="H31" s="5" t="e">
-        <f t="shared" si="6"/>
+        <f t="shared" si="12"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I31" s="9"/>
@@ -1565,7 +2489,7 @@
       <c r="L31" s="10"/>
       <c r="M31" s="11"/>
       <c r="N31" s="5" t="e">
-        <f t="shared" si="7"/>
+        <f t="shared" si="13"/>
         <v>#DIV/0!</v>
       </c>
       <c r="O31" s="9"/>
@@ -1574,11 +2498,43 @@
       <c r="R31" s="10"/>
       <c r="S31" s="11"/>
       <c r="T31" s="5" t="e">
-        <f t="shared" si="8"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
+        <f t="shared" si="14"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="U31" s="15"/>
+      <c r="V31" s="19"/>
+      <c r="W31" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="X31" s="9"/>
+      <c r="Y31" s="10"/>
+      <c r="Z31" s="10"/>
+      <c r="AA31" s="10"/>
+      <c r="AB31" s="11"/>
+      <c r="AC31" s="5" t="e">
+        <f t="shared" si="15"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AD31" s="9"/>
+      <c r="AE31" s="10"/>
+      <c r="AF31" s="10"/>
+      <c r="AG31" s="10"/>
+      <c r="AH31" s="11"/>
+      <c r="AI31" s="5" t="e">
+        <f t="shared" si="16"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AJ31" s="9"/>
+      <c r="AK31" s="10"/>
+      <c r="AL31" s="10"/>
+      <c r="AM31" s="10"/>
+      <c r="AN31" s="11"/>
+      <c r="AO31" s="5" t="e">
+        <f t="shared" si="17"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="32" spans="1:41" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="19"/>
       <c r="B32" s="4" t="s">
         <v>8</v>
@@ -1589,7 +2545,7 @@
       <c r="F32" s="10"/>
       <c r="G32" s="11"/>
       <c r="H32" s="5" t="e">
-        <f t="shared" si="6"/>
+        <f t="shared" si="12"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I32" s="9"/>
@@ -1598,7 +2554,7 @@
       <c r="L32" s="10"/>
       <c r="M32" s="11"/>
       <c r="N32" s="5" t="e">
-        <f t="shared" si="7"/>
+        <f t="shared" si="13"/>
         <v>#DIV/0!</v>
       </c>
       <c r="O32" s="9"/>
@@ -1607,11 +2563,43 @@
       <c r="R32" s="10"/>
       <c r="S32" s="11"/>
       <c r="T32" s="5" t="e">
-        <f t="shared" si="8"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="33" spans="1:20" x14ac:dyDescent="0.25">
+        <f t="shared" si="14"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="U32" s="15"/>
+      <c r="V32" s="19"/>
+      <c r="W32" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="X32" s="9"/>
+      <c r="Y32" s="10"/>
+      <c r="Z32" s="10"/>
+      <c r="AA32" s="10"/>
+      <c r="AB32" s="11"/>
+      <c r="AC32" s="5" t="e">
+        <f t="shared" si="15"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AD32" s="9"/>
+      <c r="AE32" s="10"/>
+      <c r="AF32" s="10"/>
+      <c r="AG32" s="10"/>
+      <c r="AH32" s="11"/>
+      <c r="AI32" s="5" t="e">
+        <f t="shared" si="16"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AJ32" s="9"/>
+      <c r="AK32" s="10"/>
+      <c r="AL32" s="10"/>
+      <c r="AM32" s="10"/>
+      <c r="AN32" s="11"/>
+      <c r="AO32" s="5" t="e">
+        <f t="shared" si="17"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="33" spans="1:41" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="19"/>
       <c r="B33" s="4" t="s">
         <v>9</v>
@@ -1622,7 +2610,7 @@
       <c r="F33" s="13"/>
       <c r="G33" s="14"/>
       <c r="H33" s="5" t="e">
-        <f t="shared" si="6"/>
+        <f t="shared" si="12"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I33" s="12"/>
@@ -1631,7 +2619,7 @@
       <c r="L33" s="13"/>
       <c r="M33" s="14"/>
       <c r="N33" s="5" t="e">
-        <f t="shared" si="7"/>
+        <f t="shared" si="13"/>
         <v>#DIV/0!</v>
       </c>
       <c r="O33" s="12"/>
@@ -1640,11 +2628,43 @@
       <c r="R33" s="13"/>
       <c r="S33" s="14"/>
       <c r="T33" s="5" t="e">
-        <f t="shared" si="8"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="34" spans="1:20" x14ac:dyDescent="0.25">
+        <f t="shared" si="14"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="U33" s="15"/>
+      <c r="V33" s="19"/>
+      <c r="W33" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="X33" s="12"/>
+      <c r="Y33" s="13"/>
+      <c r="Z33" s="13"/>
+      <c r="AA33" s="13"/>
+      <c r="AB33" s="14"/>
+      <c r="AC33" s="5" t="e">
+        <f t="shared" si="15"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AD33" s="12"/>
+      <c r="AE33" s="13"/>
+      <c r="AF33" s="13"/>
+      <c r="AG33" s="13"/>
+      <c r="AH33" s="14"/>
+      <c r="AI33" s="5" t="e">
+        <f t="shared" si="16"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AJ33" s="12"/>
+      <c r="AK33" s="13"/>
+      <c r="AL33" s="13"/>
+      <c r="AM33" s="13"/>
+      <c r="AN33" s="14"/>
+      <c r="AO33" s="5" t="e">
+        <f t="shared" si="17"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="34" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A34" s="18"/>
       <c r="B34" s="16"/>
       <c r="C34" s="15"/>
@@ -1665,10 +2685,31 @@
       <c r="R34" s="15"/>
       <c r="S34" s="15"/>
       <c r="T34" s="15"/>
-    </row>
-    <row r="35" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U34" s="15"/>
+      <c r="V34" s="18"/>
+      <c r="W34" s="16"/>
+      <c r="X34" s="15"/>
+      <c r="Y34" s="15"/>
+      <c r="Z34" s="15"/>
+      <c r="AA34" s="15"/>
+      <c r="AB34" s="15"/>
+      <c r="AC34" s="15"/>
+      <c r="AD34" s="15"/>
+      <c r="AE34" s="15"/>
+      <c r="AF34" s="15"/>
+      <c r="AG34" s="15"/>
+      <c r="AH34" s="15"/>
+      <c r="AI34" s="15"/>
+      <c r="AJ34" s="15"/>
+      <c r="AK34" s="15"/>
+      <c r="AL34" s="15"/>
+      <c r="AM34" s="15"/>
+      <c r="AN34" s="15"/>
+      <c r="AO34" s="15"/>
+    </row>
+    <row r="35" spans="1:41" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="19" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B35" s="4" t="s">
         <v>1</v>
@@ -1700,8 +2741,42 @@
         <f>AVERAGE(O35:S35)</f>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="36" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U35" s="15"/>
+      <c r="V35" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="W35" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="X35" s="6"/>
+      <c r="Y35" s="7"/>
+      <c r="Z35" s="7"/>
+      <c r="AA35" s="7"/>
+      <c r="AB35" s="8"/>
+      <c r="AC35" s="5" t="e">
+        <f>AVERAGE(X35:AB35)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AD35" s="6"/>
+      <c r="AE35" s="7"/>
+      <c r="AF35" s="7"/>
+      <c r="AG35" s="7"/>
+      <c r="AH35" s="8"/>
+      <c r="AI35" s="5" t="e">
+        <f>AVERAGE(AD35:AH35)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AJ35" s="6"/>
+      <c r="AK35" s="7"/>
+      <c r="AL35" s="7"/>
+      <c r="AM35" s="7"/>
+      <c r="AN35" s="8"/>
+      <c r="AO35" s="5" t="e">
+        <f>AVERAGE(AJ35:AN35)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="36" spans="1:41" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="19"/>
       <c r="B36" s="4" t="s">
         <v>2</v>
@@ -1712,7 +2787,7 @@
       <c r="F36" s="10"/>
       <c r="G36" s="11"/>
       <c r="H36" s="5" t="e">
-        <f t="shared" ref="H36:H43" si="9">AVERAGE(C36:G36)</f>
+        <f t="shared" ref="H36:H43" si="18">AVERAGE(C36:G36)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="I36" s="9"/>
@@ -1721,7 +2796,7 @@
       <c r="L36" s="10"/>
       <c r="M36" s="11"/>
       <c r="N36" s="5" t="e">
-        <f t="shared" ref="N36:N43" si="10">AVERAGE(I36:M36)</f>
+        <f t="shared" ref="N36:N43" si="19">AVERAGE(I36:M36)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="O36" s="9"/>
@@ -1730,11 +2805,43 @@
       <c r="R36" s="10"/>
       <c r="S36" s="11"/>
       <c r="T36" s="5" t="e">
-        <f t="shared" ref="T36:T43" si="11">AVERAGE(O36:S36)</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="37" spans="1:20" x14ac:dyDescent="0.25">
+        <f t="shared" ref="T36:T43" si="20">AVERAGE(O36:S36)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="U36" s="15"/>
+      <c r="V36" s="19"/>
+      <c r="W36" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="X36" s="9"/>
+      <c r="Y36" s="10"/>
+      <c r="Z36" s="10"/>
+      <c r="AA36" s="10"/>
+      <c r="AB36" s="11"/>
+      <c r="AC36" s="5" t="e">
+        <f t="shared" ref="AC36:AC43" si="21">AVERAGE(X36:AB36)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AD36" s="9"/>
+      <c r="AE36" s="10"/>
+      <c r="AF36" s="10"/>
+      <c r="AG36" s="10"/>
+      <c r="AH36" s="11"/>
+      <c r="AI36" s="5" t="e">
+        <f t="shared" ref="AI36:AI43" si="22">AVERAGE(AD36:AH36)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AJ36" s="9"/>
+      <c r="AK36" s="10"/>
+      <c r="AL36" s="10"/>
+      <c r="AM36" s="10"/>
+      <c r="AN36" s="11"/>
+      <c r="AO36" s="5" t="e">
+        <f t="shared" ref="AO36:AO43" si="23">AVERAGE(AJ36:AN36)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="37" spans="1:41" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="19"/>
       <c r="B37" s="4" t="s">
         <v>3</v>
@@ -1745,7 +2852,7 @@
       <c r="F37" s="10"/>
       <c r="G37" s="11"/>
       <c r="H37" s="5" t="e">
-        <f t="shared" si="9"/>
+        <f t="shared" si="18"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I37" s="9"/>
@@ -1754,7 +2861,7 @@
       <c r="L37" s="10"/>
       <c r="M37" s="11"/>
       <c r="N37" s="5" t="e">
-        <f t="shared" si="10"/>
+        <f t="shared" si="19"/>
         <v>#DIV/0!</v>
       </c>
       <c r="O37" s="9"/>
@@ -1763,11 +2870,43 @@
       <c r="R37" s="10"/>
       <c r="S37" s="11"/>
       <c r="T37" s="5" t="e">
-        <f t="shared" si="11"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="38" spans="1:20" x14ac:dyDescent="0.25">
+        <f t="shared" si="20"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="U37" s="15"/>
+      <c r="V37" s="19"/>
+      <c r="W37" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="X37" s="9"/>
+      <c r="Y37" s="10"/>
+      <c r="Z37" s="10"/>
+      <c r="AA37" s="10"/>
+      <c r="AB37" s="10"/>
+      <c r="AC37" s="5" t="e">
+        <f t="shared" si="21"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AD37" s="9"/>
+      <c r="AE37" s="10"/>
+      <c r="AF37" s="10"/>
+      <c r="AG37" s="10"/>
+      <c r="AH37" s="10"/>
+      <c r="AI37" s="5" t="e">
+        <f t="shared" si="22"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AJ37" s="9"/>
+      <c r="AK37" s="10"/>
+      <c r="AL37" s="10"/>
+      <c r="AM37" s="10"/>
+      <c r="AN37" s="11"/>
+      <c r="AO37" s="5" t="e">
+        <f t="shared" si="23"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="38" spans="1:41" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="19"/>
       <c r="B38" s="4" t="s">
         <v>4</v>
@@ -1778,7 +2917,7 @@
       <c r="F38" s="10"/>
       <c r="G38" s="11"/>
       <c r="H38" s="5" t="e">
-        <f t="shared" si="9"/>
+        <f t="shared" si="18"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I38" s="9"/>
@@ -1787,7 +2926,7 @@
       <c r="L38" s="10"/>
       <c r="M38" s="11"/>
       <c r="N38" s="5" t="e">
-        <f t="shared" si="10"/>
+        <f t="shared" si="19"/>
         <v>#DIV/0!</v>
       </c>
       <c r="O38" s="9"/>
@@ -1796,11 +2935,43 @@
       <c r="R38" s="10"/>
       <c r="S38" s="11"/>
       <c r="T38" s="5" t="e">
-        <f t="shared" si="11"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="39" spans="1:20" x14ac:dyDescent="0.25">
+        <f t="shared" si="20"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="U38" s="15"/>
+      <c r="V38" s="19"/>
+      <c r="W38" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="X38" s="9"/>
+      <c r="Y38" s="10"/>
+      <c r="Z38" s="10"/>
+      <c r="AA38" s="10"/>
+      <c r="AB38" s="10"/>
+      <c r="AC38" s="5" t="e">
+        <f t="shared" si="21"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AD38" s="9"/>
+      <c r="AE38" s="10"/>
+      <c r="AF38" s="10"/>
+      <c r="AG38" s="10"/>
+      <c r="AH38" s="10"/>
+      <c r="AI38" s="5" t="e">
+        <f t="shared" si="22"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AJ38" s="9"/>
+      <c r="AK38" s="10"/>
+      <c r="AL38" s="10"/>
+      <c r="AM38" s="10"/>
+      <c r="AN38" s="11"/>
+      <c r="AO38" s="5" t="e">
+        <f t="shared" si="23"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="39" spans="1:41" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="19"/>
       <c r="B39" s="4" t="s">
         <v>5</v>
@@ -1811,7 +2982,7 @@
       <c r="F39" s="10"/>
       <c r="G39" s="11"/>
       <c r="H39" s="5" t="e">
-        <f t="shared" si="9"/>
+        <f t="shared" si="18"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I39" s="9"/>
@@ -1820,7 +2991,7 @@
       <c r="L39" s="10"/>
       <c r="M39" s="11"/>
       <c r="N39" s="5" t="e">
-        <f t="shared" si="10"/>
+        <f t="shared" si="19"/>
         <v>#DIV/0!</v>
       </c>
       <c r="O39" s="9"/>
@@ -1829,11 +3000,43 @@
       <c r="R39" s="10"/>
       <c r="S39" s="11"/>
       <c r="T39" s="5" t="e">
-        <f t="shared" si="11"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="40" spans="1:20" x14ac:dyDescent="0.25">
+        <f t="shared" si="20"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="U39" s="15"/>
+      <c r="V39" s="19"/>
+      <c r="W39" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="X39" s="9"/>
+      <c r="Y39" s="10"/>
+      <c r="Z39" s="10"/>
+      <c r="AA39" s="10"/>
+      <c r="AB39" s="10"/>
+      <c r="AC39" s="5" t="e">
+        <f t="shared" si="21"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AD39" s="9"/>
+      <c r="AE39" s="10"/>
+      <c r="AF39" s="10"/>
+      <c r="AG39" s="10"/>
+      <c r="AH39" s="10"/>
+      <c r="AI39" s="5" t="e">
+        <f t="shared" si="22"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AJ39" s="9"/>
+      <c r="AK39" s="10"/>
+      <c r="AL39" s="10"/>
+      <c r="AM39" s="10"/>
+      <c r="AN39" s="11"/>
+      <c r="AO39" s="5" t="e">
+        <f t="shared" si="23"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="40" spans="1:41" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="19"/>
       <c r="B40" s="4" t="s">
         <v>6</v>
@@ -1844,7 +3047,7 @@
       <c r="F40" s="10"/>
       <c r="G40" s="11"/>
       <c r="H40" s="5" t="e">
-        <f t="shared" si="9"/>
+        <f t="shared" si="18"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I40" s="9"/>
@@ -1853,7 +3056,7 @@
       <c r="L40" s="10"/>
       <c r="M40" s="11"/>
       <c r="N40" s="5" t="e">
-        <f t="shared" si="10"/>
+        <f t="shared" si="19"/>
         <v>#DIV/0!</v>
       </c>
       <c r="O40" s="9"/>
@@ -1862,11 +3065,43 @@
       <c r="R40" s="10"/>
       <c r="S40" s="11"/>
       <c r="T40" s="5" t="e">
-        <f t="shared" si="11"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="41" spans="1:20" x14ac:dyDescent="0.25">
+        <f t="shared" si="20"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="U40" s="15"/>
+      <c r="V40" s="19"/>
+      <c r="W40" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="X40" s="9"/>
+      <c r="Y40" s="10"/>
+      <c r="Z40" s="10"/>
+      <c r="AA40" s="10"/>
+      <c r="AB40" s="11"/>
+      <c r="AC40" s="5" t="e">
+        <f t="shared" si="21"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AD40" s="9"/>
+      <c r="AE40" s="10"/>
+      <c r="AF40" s="10"/>
+      <c r="AG40" s="10"/>
+      <c r="AH40" s="11"/>
+      <c r="AI40" s="5" t="e">
+        <f t="shared" si="22"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AJ40" s="9"/>
+      <c r="AK40" s="10"/>
+      <c r="AL40" s="10"/>
+      <c r="AM40" s="10"/>
+      <c r="AN40" s="11"/>
+      <c r="AO40" s="5" t="e">
+        <f t="shared" si="23"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="41" spans="1:41" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="19"/>
       <c r="B41" s="4" t="s">
         <v>7</v>
@@ -1877,7 +3112,7 @@
       <c r="F41" s="10"/>
       <c r="G41" s="11"/>
       <c r="H41" s="5" t="e">
-        <f t="shared" si="9"/>
+        <f t="shared" si="18"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I41" s="9"/>
@@ -1886,7 +3121,7 @@
       <c r="L41" s="10"/>
       <c r="M41" s="11"/>
       <c r="N41" s="5" t="e">
-        <f t="shared" si="10"/>
+        <f t="shared" si="19"/>
         <v>#DIV/0!</v>
       </c>
       <c r="O41" s="9"/>
@@ -1895,11 +3130,43 @@
       <c r="R41" s="10"/>
       <c r="S41" s="11"/>
       <c r="T41" s="5" t="e">
-        <f t="shared" si="11"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="42" spans="1:20" x14ac:dyDescent="0.25">
+        <f t="shared" si="20"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="U41" s="15"/>
+      <c r="V41" s="19"/>
+      <c r="W41" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="X41" s="9"/>
+      <c r="Y41" s="10"/>
+      <c r="Z41" s="10"/>
+      <c r="AA41" s="10"/>
+      <c r="AB41" s="11"/>
+      <c r="AC41" s="5" t="e">
+        <f t="shared" si="21"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AD41" s="9"/>
+      <c r="AE41" s="10"/>
+      <c r="AF41" s="10"/>
+      <c r="AG41" s="10"/>
+      <c r="AH41" s="11"/>
+      <c r="AI41" s="5" t="e">
+        <f t="shared" si="22"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AJ41" s="9"/>
+      <c r="AK41" s="10"/>
+      <c r="AL41" s="10"/>
+      <c r="AM41" s="10"/>
+      <c r="AN41" s="11"/>
+      <c r="AO41" s="5" t="e">
+        <f t="shared" si="23"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="42" spans="1:41" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="19"/>
       <c r="B42" s="4" t="s">
         <v>8</v>
@@ -1910,7 +3177,7 @@
       <c r="F42" s="10"/>
       <c r="G42" s="11"/>
       <c r="H42" s="5" t="e">
-        <f t="shared" si="9"/>
+        <f t="shared" si="18"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I42" s="9"/>
@@ -1919,7 +3186,7 @@
       <c r="L42" s="10"/>
       <c r="M42" s="11"/>
       <c r="N42" s="5" t="e">
-        <f t="shared" si="10"/>
+        <f t="shared" si="19"/>
         <v>#DIV/0!</v>
       </c>
       <c r="O42" s="9"/>
@@ -1928,11 +3195,43 @@
       <c r="R42" s="10"/>
       <c r="S42" s="11"/>
       <c r="T42" s="5" t="e">
-        <f t="shared" si="11"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="43" spans="1:20" x14ac:dyDescent="0.25">
+        <f t="shared" si="20"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="U42" s="15"/>
+      <c r="V42" s="19"/>
+      <c r="W42" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="X42" s="9"/>
+      <c r="Y42" s="10"/>
+      <c r="Z42" s="10"/>
+      <c r="AA42" s="10"/>
+      <c r="AB42" s="11"/>
+      <c r="AC42" s="5" t="e">
+        <f t="shared" si="21"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AD42" s="9"/>
+      <c r="AE42" s="10"/>
+      <c r="AF42" s="10"/>
+      <c r="AG42" s="10"/>
+      <c r="AH42" s="11"/>
+      <c r="AI42" s="5" t="e">
+        <f t="shared" si="22"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AJ42" s="9"/>
+      <c r="AK42" s="10"/>
+      <c r="AL42" s="10"/>
+      <c r="AM42" s="10"/>
+      <c r="AN42" s="11"/>
+      <c r="AO42" s="5" t="e">
+        <f t="shared" si="23"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="43" spans="1:41" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="19"/>
       <c r="B43" s="4" t="s">
         <v>9</v>
@@ -1943,7 +3242,7 @@
       <c r="F43" s="13"/>
       <c r="G43" s="14"/>
       <c r="H43" s="5" t="e">
-        <f t="shared" si="9"/>
+        <f t="shared" si="18"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I43" s="12"/>
@@ -1952,7 +3251,7 @@
       <c r="L43" s="13"/>
       <c r="M43" s="14"/>
       <c r="N43" s="5" t="e">
-        <f t="shared" si="10"/>
+        <f t="shared" si="19"/>
         <v>#DIV/0!</v>
       </c>
       <c r="O43" s="12"/>
@@ -1961,27 +3260,59 @@
       <c r="R43" s="13"/>
       <c r="S43" s="14"/>
       <c r="T43" s="5" t="e">
-        <f t="shared" si="11"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="44" spans="1:20" x14ac:dyDescent="0.25">
+        <f t="shared" si="20"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="U43" s="15"/>
+      <c r="V43" s="19"/>
+      <c r="W43" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="X43" s="12"/>
+      <c r="Y43" s="13"/>
+      <c r="Z43" s="13"/>
+      <c r="AA43" s="13"/>
+      <c r="AB43" s="14"/>
+      <c r="AC43" s="5" t="e">
+        <f t="shared" si="21"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AD43" s="12"/>
+      <c r="AE43" s="13"/>
+      <c r="AF43" s="13"/>
+      <c r="AG43" s="13"/>
+      <c r="AH43" s="14"/>
+      <c r="AI43" s="5" t="e">
+        <f t="shared" si="22"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AJ43" s="12"/>
+      <c r="AK43" s="13"/>
+      <c r="AL43" s="13"/>
+      <c r="AM43" s="13"/>
+      <c r="AN43" s="14"/>
+      <c r="AO43" s="5" t="e">
+        <f t="shared" si="23"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="44" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A44"/>
       <c r="B44"/>
     </row>
-    <row r="45" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A45"/>
       <c r="B45"/>
     </row>
-    <row r="46" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A46"/>
       <c r="B46"/>
     </row>
-    <row r="47" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A47"/>
       <c r="B47"/>
     </row>
-    <row r="48" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A48"/>
       <c r="B48"/>
     </row>
@@ -2125,40 +3456,24 @@
       <c r="A83"/>
       <c r="B83"/>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A84"/>
-      <c r="B84"/>
-    </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A85"/>
-      <c r="B85"/>
-    </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A86"/>
-      <c r="B86"/>
-    </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A87"/>
-      <c r="B87"/>
-    </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A88"/>
-      <c r="B88"/>
-    </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A89"/>
-      <c r="B89"/>
-    </row>
   </sheetData>
-  <mergeCells count="8">
-    <mergeCell ref="O3:T3"/>
-    <mergeCell ref="A15:A23"/>
+  <mergeCells count="16">
     <mergeCell ref="A1:C2"/>
     <mergeCell ref="A5:A13"/>
     <mergeCell ref="C3:H3"/>
     <mergeCell ref="I3:N3"/>
+    <mergeCell ref="AD3:AI3"/>
+    <mergeCell ref="AJ3:AO3"/>
+    <mergeCell ref="V5:V13"/>
     <mergeCell ref="A25:A33"/>
     <mergeCell ref="A35:A43"/>
+    <mergeCell ref="O3:T3"/>
+    <mergeCell ref="A15:A23"/>
+    <mergeCell ref="V15:V23"/>
+    <mergeCell ref="V25:V33"/>
+    <mergeCell ref="V35:V43"/>
+    <mergeCell ref="V1:X2"/>
+    <mergeCell ref="X3:AC3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Aggiunti primi tempi per bf2 su GTX1070
</commit_message>
<xml_diff>
--- a/performance bf2.xlsx
+++ b/performance bf2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Filippo\Desktop\tesi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B8EF593-4E89-4799-A58B-B5188342FFF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD0E19FE-3320-4C34-8D13-AB719E19A79F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="26">
   <si>
     <t>SPEEDUP</t>
   </si>
@@ -106,6 +106,12 @@
   </si>
   <si>
     <t>bf2-soa-sh</t>
+  </si>
+  <si>
+    <t>&gt;1h</t>
+  </si>
+  <si>
+    <t>N/A</t>
   </si>
 </sst>
 </file>
@@ -310,11 +316,11 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -601,8 +607,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AO83"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AD9" sqref="AD9"/>
+    <sheetView tabSelected="1" topLeftCell="U1" workbookViewId="0">
+      <selection activeCell="AE31" sqref="AE31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -613,25 +619,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="V1" s="20" t="s">
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="V1" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="W1" s="20"/>
-      <c r="X1" s="20"/>
+      <c r="W1" s="19"/>
+      <c r="X1" s="19"/>
     </row>
     <row r="2" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A2" s="20"/>
-      <c r="B2" s="20"/>
-      <c r="C2" s="20"/>
+      <c r="A2" s="19"/>
+      <c r="B2" s="19"/>
+      <c r="C2" s="19"/>
       <c r="U2" s="15"/>
-      <c r="V2" s="20"/>
-      <c r="W2" s="20"/>
-      <c r="X2" s="20"/>
+      <c r="V2" s="19"/>
+      <c r="W2" s="19"/>
+      <c r="X2" s="19"/>
     </row>
     <row r="3" spans="1:41" ht="18.75" x14ac:dyDescent="0.25">
       <c r="C3" s="21" t="s">
@@ -800,7 +806,7 @@
       </c>
     </row>
     <row r="5" spans="1:41" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="19" t="s">
+      <c r="A5" s="20" t="s">
         <v>20</v>
       </c>
       <c r="B5" s="4" t="s">
@@ -834,7 +840,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="U5" s="15"/>
-      <c r="V5" s="19" t="s">
+      <c r="V5" s="20" t="s">
         <v>20</v>
       </c>
       <c r="W5" s="4" t="s">
@@ -869,7 +875,7 @@
       </c>
     </row>
     <row r="6" spans="1:41" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="19"/>
+      <c r="A6" s="20"/>
       <c r="B6" s="4" t="s">
         <v>2</v>
       </c>
@@ -903,7 +909,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="U6" s="15"/>
-      <c r="V6" s="19"/>
+      <c r="V6" s="20"/>
       <c r="W6" s="4" t="s">
         <v>2</v>
       </c>
@@ -938,7 +944,7 @@
       </c>
     </row>
     <row r="7" spans="1:41" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="19"/>
+      <c r="A7" s="20"/>
       <c r="B7" s="4" t="s">
         <v>3</v>
       </c>
@@ -972,7 +978,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="U7" s="15"/>
-      <c r="V7" s="19"/>
+      <c r="V7" s="20"/>
       <c r="W7" s="4" t="s">
         <v>3</v>
       </c>
@@ -1007,7 +1013,7 @@
       </c>
     </row>
     <row r="8" spans="1:41" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="19"/>
+      <c r="A8" s="20"/>
       <c r="B8" s="4" t="s">
         <v>4</v>
       </c>
@@ -1041,7 +1047,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="U8" s="15"/>
-      <c r="V8" s="19"/>
+      <c r="V8" s="20"/>
       <c r="W8" s="4" t="s">
         <v>4</v>
       </c>
@@ -1076,7 +1082,7 @@
       </c>
     </row>
     <row r="9" spans="1:41" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="19"/>
+      <c r="A9" s="20"/>
       <c r="B9" s="4" t="s">
         <v>5</v>
       </c>
@@ -1089,7 +1095,9 @@
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="I9" s="9"/>
+      <c r="I9" s="9" t="s">
+        <v>24</v>
+      </c>
       <c r="J9" s="10"/>
       <c r="K9" s="10"/>
       <c r="L9" s="10"/>
@@ -1108,7 +1116,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="U9" s="15"/>
-      <c r="V9" s="19"/>
+      <c r="V9" s="20"/>
       <c r="W9" s="4" t="s">
         <v>5</v>
       </c>
@@ -1121,11 +1129,21 @@
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="AD9" s="9"/>
-      <c r="AE9" s="10"/>
-      <c r="AF9" s="10"/>
-      <c r="AG9" s="10"/>
-      <c r="AH9" s="10"/>
+      <c r="AD9" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="AE9" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="AF9" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="AG9" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="AH9" s="10" t="s">
+        <v>25</v>
+      </c>
       <c r="AI9" s="5" t="e">
         <f t="shared" si="4"/>
         <v>#DIV/0!</v>
@@ -1141,7 +1159,7 @@
       </c>
     </row>
     <row r="10" spans="1:41" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="19"/>
+      <c r="A10" s="20"/>
       <c r="B10" s="4" t="s">
         <v>6</v>
       </c>
@@ -1173,7 +1191,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="U10" s="15"/>
-      <c r="V10" s="19"/>
+      <c r="V10" s="20"/>
       <c r="W10" s="4" t="s">
         <v>6</v>
       </c>
@@ -1206,7 +1224,7 @@
       </c>
     </row>
     <row r="11" spans="1:41" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="19"/>
+      <c r="A11" s="20"/>
       <c r="B11" s="4" t="s">
         <v>7</v>
       </c>
@@ -1238,7 +1256,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="U11" s="15"/>
-      <c r="V11" s="19"/>
+      <c r="V11" s="20"/>
       <c r="W11" s="4" t="s">
         <v>7</v>
       </c>
@@ -1271,7 +1289,7 @@
       </c>
     </row>
     <row r="12" spans="1:41" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="19"/>
+      <c r="A12" s="20"/>
       <c r="B12" s="4" t="s">
         <v>8</v>
       </c>
@@ -1303,7 +1321,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="U12" s="15"/>
-      <c r="V12" s="19"/>
+      <c r="V12" s="20"/>
       <c r="W12" s="4" t="s">
         <v>8</v>
       </c>
@@ -1336,7 +1354,7 @@
       </c>
     </row>
     <row r="13" spans="1:41" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="19"/>
+      <c r="A13" s="20"/>
       <c r="B13" s="4" t="s">
         <v>9</v>
       </c>
@@ -1368,7 +1386,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="U13" s="15"/>
-      <c r="V13" s="19"/>
+      <c r="V13" s="20"/>
       <c r="W13" s="4" t="s">
         <v>9</v>
       </c>
@@ -1444,7 +1462,7 @@
       <c r="AO14" s="15"/>
     </row>
     <row r="15" spans="1:41" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="19" t="s">
+      <c r="A15" s="20" t="s">
         <v>21</v>
       </c>
       <c r="B15" s="4" t="s">
@@ -1478,7 +1496,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="U15" s="15"/>
-      <c r="V15" s="19" t="s">
+      <c r="V15" s="20" t="s">
         <v>21</v>
       </c>
       <c r="W15" s="4" t="s">
@@ -1513,7 +1531,7 @@
       </c>
     </row>
     <row r="16" spans="1:41" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="19"/>
+      <c r="A16" s="20"/>
       <c r="B16" s="4" t="s">
         <v>2</v>
       </c>
@@ -1526,14 +1544,16 @@
         <f t="shared" ref="H16:H23" si="6">AVERAGE(C16:G16)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="I16" s="9"/>
+      <c r="I16" s="9">
+        <v>101.76300000000001</v>
+      </c>
       <c r="J16" s="10"/>
       <c r="K16" s="10"/>
       <c r="L16" s="10"/>
       <c r="M16" s="11"/>
-      <c r="N16" s="5" t="e">
+      <c r="N16" s="5">
         <f t="shared" ref="N16:N23" si="7">AVERAGE(I16:M16)</f>
-        <v>#DIV/0!</v>
+        <v>101.76300000000001</v>
       </c>
       <c r="O16" s="9"/>
       <c r="P16" s="10"/>
@@ -1545,7 +1565,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="U16" s="15"/>
-      <c r="V16" s="19"/>
+      <c r="V16" s="20"/>
       <c r="W16" s="4" t="s">
         <v>2</v>
       </c>
@@ -1558,14 +1578,16 @@
         <f t="shared" ref="AC16:AC23" si="9">AVERAGE(X16:AB16)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="AD16" s="9"/>
+      <c r="AD16" s="9">
+        <v>57.79</v>
+      </c>
       <c r="AE16" s="10"/>
       <c r="AF16" s="10"/>
       <c r="AG16" s="10"/>
       <c r="AH16" s="11"/>
-      <c r="AI16" s="5" t="e">
+      <c r="AI16" s="5">
         <f t="shared" ref="AI16:AI23" si="10">AVERAGE(AD16:AH16)</f>
-        <v>#DIV/0!</v>
+        <v>57.79</v>
       </c>
       <c r="AJ16" s="9"/>
       <c r="AK16" s="10"/>
@@ -1578,7 +1600,7 @@
       </c>
     </row>
     <row r="17" spans="1:41" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="19"/>
+      <c r="A17" s="20"/>
       <c r="B17" s="4" t="s">
         <v>3</v>
       </c>
@@ -1591,14 +1613,16 @@
         <f t="shared" si="6"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="I17" s="9"/>
+      <c r="I17" s="9">
+        <v>397.11799999999999</v>
+      </c>
       <c r="J17" s="10"/>
       <c r="K17" s="10"/>
       <c r="L17" s="10"/>
       <c r="M17" s="11"/>
-      <c r="N17" s="5" t="e">
+      <c r="N17" s="5">
         <f t="shared" si="7"/>
-        <v>#DIV/0!</v>
+        <v>397.11799999999999</v>
       </c>
       <c r="O17" s="9"/>
       <c r="P17" s="10"/>
@@ -1610,7 +1634,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="U17" s="15"/>
-      <c r="V17" s="19"/>
+      <c r="V17" s="20"/>
       <c r="W17" s="4" t="s">
         <v>3</v>
       </c>
@@ -1623,14 +1647,16 @@
         <f t="shared" si="9"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="AD17" s="9"/>
+      <c r="AD17" s="9">
+        <v>52.55</v>
+      </c>
       <c r="AE17" s="10"/>
       <c r="AF17" s="10"/>
       <c r="AG17" s="10"/>
       <c r="AH17" s="10"/>
-      <c r="AI17" s="5" t="e">
+      <c r="AI17" s="5">
         <f t="shared" si="10"/>
-        <v>#DIV/0!</v>
+        <v>52.55</v>
       </c>
       <c r="AJ17" s="9"/>
       <c r="AK17" s="10"/>
@@ -1643,7 +1669,7 @@
       </c>
     </row>
     <row r="18" spans="1:41" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="19"/>
+      <c r="A18" s="20"/>
       <c r="B18" s="4" t="s">
         <v>4</v>
       </c>
@@ -1656,14 +1682,16 @@
         <f t="shared" si="6"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="I18" s="9"/>
+      <c r="I18" s="9">
+        <v>1564.66</v>
+      </c>
       <c r="J18" s="10"/>
       <c r="K18" s="10"/>
       <c r="L18" s="10"/>
       <c r="M18" s="11"/>
-      <c r="N18" s="5" t="e">
+      <c r="N18" s="5">
         <f t="shared" si="7"/>
-        <v>#DIV/0!</v>
+        <v>1564.66</v>
       </c>
       <c r="O18" s="9"/>
       <c r="P18" s="10"/>
@@ -1675,7 +1703,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="U18" s="15"/>
-      <c r="V18" s="19"/>
+      <c r="V18" s="20"/>
       <c r="W18" s="4" t="s">
         <v>4</v>
       </c>
@@ -1688,14 +1716,16 @@
         <f t="shared" si="9"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="AD18" s="9"/>
+      <c r="AD18" s="9">
+        <v>52.92</v>
+      </c>
       <c r="AE18" s="10"/>
       <c r="AF18" s="10"/>
       <c r="AG18" s="10"/>
       <c r="AH18" s="10"/>
-      <c r="AI18" s="5" t="e">
+      <c r="AI18" s="5">
         <f t="shared" si="10"/>
-        <v>#DIV/0!</v>
+        <v>52.92</v>
       </c>
       <c r="AJ18" s="9"/>
       <c r="AK18" s="10"/>
@@ -1708,7 +1738,7 @@
       </c>
     </row>
     <row r="19" spans="1:41" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="19"/>
+      <c r="A19" s="20"/>
       <c r="B19" s="4" t="s">
         <v>5</v>
       </c>
@@ -1721,7 +1751,9 @@
         <f t="shared" si="6"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="I19" s="9"/>
+      <c r="I19" s="9" t="s">
+        <v>24</v>
+      </c>
       <c r="J19" s="10"/>
       <c r="K19" s="10"/>
       <c r="L19" s="10"/>
@@ -1740,7 +1772,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="U19" s="15"/>
-      <c r="V19" s="19"/>
+      <c r="V19" s="20"/>
       <c r="W19" s="4" t="s">
         <v>5</v>
       </c>
@@ -1753,11 +1785,21 @@
         <f t="shared" si="9"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="AD19" s="9"/>
-      <c r="AE19" s="10"/>
-      <c r="AF19" s="10"/>
-      <c r="AG19" s="10"/>
-      <c r="AH19" s="10"/>
+      <c r="AD19" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="AE19" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="AF19" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="AG19" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="AH19" s="10" t="s">
+        <v>25</v>
+      </c>
       <c r="AI19" s="5" t="e">
         <f t="shared" si="10"/>
         <v>#DIV/0!</v>
@@ -1773,7 +1815,7 @@
       </c>
     </row>
     <row r="20" spans="1:41" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="19"/>
+      <c r="A20" s="20"/>
       <c r="B20" s="4" t="s">
         <v>6</v>
       </c>
@@ -1805,7 +1847,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="U20" s="15"/>
-      <c r="V20" s="19"/>
+      <c r="V20" s="20"/>
       <c r="W20" s="4" t="s">
         <v>6</v>
       </c>
@@ -1838,7 +1880,7 @@
       </c>
     </row>
     <row r="21" spans="1:41" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="19"/>
+      <c r="A21" s="20"/>
       <c r="B21" s="4" t="s">
         <v>7</v>
       </c>
@@ -1870,7 +1912,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="U21" s="15"/>
-      <c r="V21" s="19"/>
+      <c r="V21" s="20"/>
       <c r="W21" s="4" t="s">
         <v>7</v>
       </c>
@@ -1903,7 +1945,7 @@
       </c>
     </row>
     <row r="22" spans="1:41" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="19"/>
+      <c r="A22" s="20"/>
       <c r="B22" s="4" t="s">
         <v>8</v>
       </c>
@@ -1935,7 +1977,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="U22" s="15"/>
-      <c r="V22" s="19"/>
+      <c r="V22" s="20"/>
       <c r="W22" s="4" t="s">
         <v>8</v>
       </c>
@@ -1968,7 +2010,7 @@
       </c>
     </row>
     <row r="23" spans="1:41" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="19"/>
+      <c r="A23" s="20"/>
       <c r="B23" s="4" t="s">
         <v>9</v>
       </c>
@@ -2000,7 +2042,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="U23" s="15"/>
-      <c r="V23" s="19"/>
+      <c r="V23" s="20"/>
       <c r="W23" s="4" t="s">
         <v>9</v>
       </c>
@@ -2076,7 +2118,7 @@
       <c r="AO24" s="15"/>
     </row>
     <row r="25" spans="1:41" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="19" t="s">
+      <c r="A25" s="20" t="s">
         <v>22</v>
       </c>
       <c r="B25" s="4" t="s">
@@ -2110,7 +2152,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="U25" s="15"/>
-      <c r="V25" s="19" t="s">
+      <c r="V25" s="20" t="s">
         <v>22</v>
       </c>
       <c r="W25" s="4" t="s">
@@ -2145,7 +2187,7 @@
       </c>
     </row>
     <row r="26" spans="1:41" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="19"/>
+      <c r="A26" s="20"/>
       <c r="B26" s="4" t="s">
         <v>2</v>
       </c>
@@ -2158,14 +2200,16 @@
         <f t="shared" ref="H26:H33" si="12">AVERAGE(C26:G26)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="I26" s="9"/>
+      <c r="I26" s="9">
+        <v>64.331999999999994</v>
+      </c>
       <c r="J26" s="10"/>
       <c r="K26" s="10"/>
       <c r="L26" s="10"/>
       <c r="M26" s="11"/>
-      <c r="N26" s="5" t="e">
+      <c r="N26" s="5">
         <f t="shared" ref="N26:N33" si="13">AVERAGE(I26:M26)</f>
-        <v>#DIV/0!</v>
+        <v>64.331999999999994</v>
       </c>
       <c r="O26" s="9"/>
       <c r="P26" s="10"/>
@@ -2177,7 +2221,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="U26" s="15"/>
-      <c r="V26" s="19"/>
+      <c r="V26" s="20"/>
       <c r="W26" s="4" t="s">
         <v>2</v>
       </c>
@@ -2190,14 +2234,16 @@
         <f t="shared" ref="AC26:AC33" si="15">AVERAGE(X26:AB26)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="AD26" s="9"/>
+      <c r="AD26" s="9">
+        <v>91.41</v>
+      </c>
       <c r="AE26" s="10"/>
       <c r="AF26" s="10"/>
       <c r="AG26" s="10"/>
       <c r="AH26" s="11"/>
-      <c r="AI26" s="5" t="e">
+      <c r="AI26" s="5">
         <f t="shared" ref="AI26:AI33" si="16">AVERAGE(AD26:AH26)</f>
-        <v>#DIV/0!</v>
+        <v>91.41</v>
       </c>
       <c r="AJ26" s="9"/>
       <c r="AK26" s="10"/>
@@ -2210,7 +2256,7 @@
       </c>
     </row>
     <row r="27" spans="1:41" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="19"/>
+      <c r="A27" s="20"/>
       <c r="B27" s="4" t="s">
         <v>3</v>
       </c>
@@ -2223,14 +2269,16 @@
         <f t="shared" si="12"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="I27" s="9"/>
+      <c r="I27" s="9">
+        <v>368.23700000000002</v>
+      </c>
       <c r="J27" s="10"/>
       <c r="K27" s="10"/>
       <c r="L27" s="10"/>
       <c r="M27" s="11"/>
-      <c r="N27" s="5" t="e">
+      <c r="N27" s="5">
         <f t="shared" si="13"/>
-        <v>#DIV/0!</v>
+        <v>368.23700000000002</v>
       </c>
       <c r="O27" s="9"/>
       <c r="P27" s="10"/>
@@ -2242,7 +2290,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="U27" s="15"/>
-      <c r="V27" s="19"/>
+      <c r="V27" s="20"/>
       <c r="W27" s="4" t="s">
         <v>3</v>
       </c>
@@ -2255,14 +2303,16 @@
         <f t="shared" si="15"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="AD27" s="9"/>
+      <c r="AD27" s="9">
+        <v>56.67</v>
+      </c>
       <c r="AE27" s="10"/>
       <c r="AF27" s="10"/>
       <c r="AG27" s="10"/>
       <c r="AH27" s="10"/>
-      <c r="AI27" s="5" t="e">
+      <c r="AI27" s="5">
         <f t="shared" si="16"/>
-        <v>#DIV/0!</v>
+        <v>56.67</v>
       </c>
       <c r="AJ27" s="9"/>
       <c r="AK27" s="10"/>
@@ -2275,7 +2325,7 @@
       </c>
     </row>
     <row r="28" spans="1:41" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="19"/>
+      <c r="A28" s="20"/>
       <c r="B28" s="4" t="s">
         <v>4</v>
       </c>
@@ -2288,14 +2338,16 @@
         <f t="shared" si="12"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="I28" s="9"/>
+      <c r="I28" s="9">
+        <v>1448.54</v>
+      </c>
       <c r="J28" s="10"/>
       <c r="K28" s="10"/>
       <c r="L28" s="10"/>
       <c r="M28" s="11"/>
-      <c r="N28" s="5" t="e">
+      <c r="N28" s="5">
         <f t="shared" si="13"/>
-        <v>#DIV/0!</v>
+        <v>1448.54</v>
       </c>
       <c r="O28" s="9"/>
       <c r="P28" s="10"/>
@@ -2307,7 +2359,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="U28" s="15"/>
-      <c r="V28" s="19"/>
+      <c r="V28" s="20"/>
       <c r="W28" s="4" t="s">
         <v>4</v>
       </c>
@@ -2320,14 +2372,16 @@
         <f t="shared" si="15"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="AD28" s="9"/>
+      <c r="AD28" s="9">
+        <v>57.16</v>
+      </c>
       <c r="AE28" s="10"/>
       <c r="AF28" s="10"/>
       <c r="AG28" s="10"/>
       <c r="AH28" s="10"/>
-      <c r="AI28" s="5" t="e">
+      <c r="AI28" s="5">
         <f t="shared" si="16"/>
-        <v>#DIV/0!</v>
+        <v>57.16</v>
       </c>
       <c r="AJ28" s="9"/>
       <c r="AK28" s="10"/>
@@ -2340,7 +2394,7 @@
       </c>
     </row>
     <row r="29" spans="1:41" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="19"/>
+      <c r="A29" s="20"/>
       <c r="B29" s="4" t="s">
         <v>5</v>
       </c>
@@ -2353,7 +2407,9 @@
         <f t="shared" si="12"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="I29" s="9"/>
+      <c r="I29" s="9" t="s">
+        <v>24</v>
+      </c>
       <c r="J29" s="10"/>
       <c r="K29" s="10"/>
       <c r="L29" s="10"/>
@@ -2372,7 +2428,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="U29" s="15"/>
-      <c r="V29" s="19"/>
+      <c r="V29" s="20"/>
       <c r="W29" s="4" t="s">
         <v>5</v>
       </c>
@@ -2385,11 +2441,21 @@
         <f t="shared" si="15"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="AD29" s="9"/>
-      <c r="AE29" s="10"/>
-      <c r="AF29" s="10"/>
-      <c r="AG29" s="10"/>
-      <c r="AH29" s="10"/>
+      <c r="AD29" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="AE29" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="AF29" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="AG29" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="AH29" s="10" t="s">
+        <v>25</v>
+      </c>
       <c r="AI29" s="5" t="e">
         <f t="shared" si="16"/>
         <v>#DIV/0!</v>
@@ -2405,7 +2471,7 @@
       </c>
     </row>
     <row r="30" spans="1:41" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="19"/>
+      <c r="A30" s="20"/>
       <c r="B30" s="4" t="s">
         <v>6</v>
       </c>
@@ -2437,7 +2503,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="U30" s="15"/>
-      <c r="V30" s="19"/>
+      <c r="V30" s="20"/>
       <c r="W30" s="4" t="s">
         <v>6</v>
       </c>
@@ -2470,7 +2536,7 @@
       </c>
     </row>
     <row r="31" spans="1:41" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="19"/>
+      <c r="A31" s="20"/>
       <c r="B31" s="4" t="s">
         <v>7</v>
       </c>
@@ -2502,7 +2568,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="U31" s="15"/>
-      <c r="V31" s="19"/>
+      <c r="V31" s="20"/>
       <c r="W31" s="4" t="s">
         <v>7</v>
       </c>
@@ -2535,7 +2601,7 @@
       </c>
     </row>
     <row r="32" spans="1:41" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="19"/>
+      <c r="A32" s="20"/>
       <c r="B32" s="4" t="s">
         <v>8</v>
       </c>
@@ -2567,7 +2633,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="U32" s="15"/>
-      <c r="V32" s="19"/>
+      <c r="V32" s="20"/>
       <c r="W32" s="4" t="s">
         <v>8</v>
       </c>
@@ -2600,7 +2666,7 @@
       </c>
     </row>
     <row r="33" spans="1:41" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="19"/>
+      <c r="A33" s="20"/>
       <c r="B33" s="4" t="s">
         <v>9</v>
       </c>
@@ -2632,7 +2698,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="U33" s="15"/>
-      <c r="V33" s="19"/>
+      <c r="V33" s="20"/>
       <c r="W33" s="4" t="s">
         <v>9</v>
       </c>
@@ -2708,7 +2774,7 @@
       <c r="AO34" s="15"/>
     </row>
     <row r="35" spans="1:41" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="19" t="s">
+      <c r="A35" s="20" t="s">
         <v>23</v>
       </c>
       <c r="B35" s="4" t="s">
@@ -2742,7 +2808,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="U35" s="15"/>
-      <c r="V35" s="19" t="s">
+      <c r="V35" s="20" t="s">
         <v>23</v>
       </c>
       <c r="W35" s="4" t="s">
@@ -2777,7 +2843,7 @@
       </c>
     </row>
     <row r="36" spans="1:41" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="19"/>
+      <c r="A36" s="20"/>
       <c r="B36" s="4" t="s">
         <v>2</v>
       </c>
@@ -2809,7 +2875,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="U36" s="15"/>
-      <c r="V36" s="19"/>
+      <c r="V36" s="20"/>
       <c r="W36" s="4" t="s">
         <v>2</v>
       </c>
@@ -2842,7 +2908,7 @@
       </c>
     </row>
     <row r="37" spans="1:41" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="19"/>
+      <c r="A37" s="20"/>
       <c r="B37" s="4" t="s">
         <v>3</v>
       </c>
@@ -2874,7 +2940,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="U37" s="15"/>
-      <c r="V37" s="19"/>
+      <c r="V37" s="20"/>
       <c r="W37" s="4" t="s">
         <v>3</v>
       </c>
@@ -2907,7 +2973,7 @@
       </c>
     </row>
     <row r="38" spans="1:41" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="19"/>
+      <c r="A38" s="20"/>
       <c r="B38" s="4" t="s">
         <v>4</v>
       </c>
@@ -2939,7 +3005,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="U38" s="15"/>
-      <c r="V38" s="19"/>
+      <c r="V38" s="20"/>
       <c r="W38" s="4" t="s">
         <v>4</v>
       </c>
@@ -2972,7 +3038,7 @@
       </c>
     </row>
     <row r="39" spans="1:41" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="19"/>
+      <c r="A39" s="20"/>
       <c r="B39" s="4" t="s">
         <v>5</v>
       </c>
@@ -3004,7 +3070,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="U39" s="15"/>
-      <c r="V39" s="19"/>
+      <c r="V39" s="20"/>
       <c r="W39" s="4" t="s">
         <v>5</v>
       </c>
@@ -3037,7 +3103,7 @@
       </c>
     </row>
     <row r="40" spans="1:41" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="19"/>
+      <c r="A40" s="20"/>
       <c r="B40" s="4" t="s">
         <v>6</v>
       </c>
@@ -3069,7 +3135,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="U40" s="15"/>
-      <c r="V40" s="19"/>
+      <c r="V40" s="20"/>
       <c r="W40" s="4" t="s">
         <v>6</v>
       </c>
@@ -3102,7 +3168,7 @@
       </c>
     </row>
     <row r="41" spans="1:41" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="19"/>
+      <c r="A41" s="20"/>
       <c r="B41" s="4" t="s">
         <v>7</v>
       </c>
@@ -3134,7 +3200,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="U41" s="15"/>
-      <c r="V41" s="19"/>
+      <c r="V41" s="20"/>
       <c r="W41" s="4" t="s">
         <v>7</v>
       </c>
@@ -3167,7 +3233,7 @@
       </c>
     </row>
     <row r="42" spans="1:41" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="19"/>
+      <c r="A42" s="20"/>
       <c r="B42" s="4" t="s">
         <v>8</v>
       </c>
@@ -3199,7 +3265,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="U42" s="15"/>
-      <c r="V42" s="19"/>
+      <c r="V42" s="20"/>
       <c r="W42" s="4" t="s">
         <v>8</v>
       </c>
@@ -3232,7 +3298,7 @@
       </c>
     </row>
     <row r="43" spans="1:41" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="19"/>
+      <c r="A43" s="20"/>
       <c r="B43" s="4" t="s">
         <v>9</v>
       </c>
@@ -3264,7 +3330,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="U43" s="15"/>
-      <c r="V43" s="19"/>
+      <c r="V43" s="20"/>
       <c r="W43" s="4" t="s">
         <v>9</v>
       </c>
@@ -3458,11 +3524,6 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="A1:C2"/>
-    <mergeCell ref="A5:A13"/>
-    <mergeCell ref="C3:H3"/>
-    <mergeCell ref="I3:N3"/>
-    <mergeCell ref="AD3:AI3"/>
     <mergeCell ref="AJ3:AO3"/>
     <mergeCell ref="V5:V13"/>
     <mergeCell ref="A25:A33"/>
@@ -3472,8 +3533,13 @@
     <mergeCell ref="V15:V23"/>
     <mergeCell ref="V25:V33"/>
     <mergeCell ref="V35:V43"/>
+    <mergeCell ref="X3:AC3"/>
+    <mergeCell ref="A1:C2"/>
+    <mergeCell ref="A5:A13"/>
+    <mergeCell ref="C3:H3"/>
+    <mergeCell ref="I3:N3"/>
+    <mergeCell ref="AD3:AI3"/>
     <mergeCell ref="V1:X2"/>
-    <mergeCell ref="X3:AC3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Aggiunti altri valori per graph-DE e bf2 su GTX1070
</commit_message>
<xml_diff>
--- a/performance bf2.xlsx
+++ b/performance bf2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Filippo\Desktop\tesi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD0E19FE-3320-4C34-8D13-AB719E19A79F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D7F3029-DF7A-47A0-A214-62E0F18FC27F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2295" yWindow="2295" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -286,7 +286,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -316,13 +316,14 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -607,8 +608,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AO83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="U1" workbookViewId="0">
-      <selection activeCell="AE31" sqref="AE31"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="AI26" sqref="AI26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -619,78 +620,78 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="V1" s="19" t="s">
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="V1" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="W1" s="19"/>
-      <c r="X1" s="19"/>
+      <c r="W1" s="22"/>
+      <c r="X1" s="22"/>
     </row>
     <row r="2" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A2" s="19"/>
-      <c r="B2" s="19"/>
-      <c r="C2" s="19"/>
+      <c r="A2" s="22"/>
+      <c r="B2" s="22"/>
+      <c r="C2" s="22"/>
       <c r="U2" s="15"/>
-      <c r="V2" s="19"/>
-      <c r="W2" s="19"/>
-      <c r="X2" s="19"/>
+      <c r="V2" s="22"/>
+      <c r="W2" s="22"/>
+      <c r="X2" s="22"/>
     </row>
     <row r="3" spans="1:41" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="C3" s="21" t="s">
+      <c r="C3" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="21"/>
-      <c r="E3" s="21"/>
-      <c r="F3" s="21"/>
-      <c r="G3" s="21"/>
-      <c r="H3" s="21"/>
-      <c r="I3" s="21" t="s">
+      <c r="D3" s="20"/>
+      <c r="E3" s="20"/>
+      <c r="F3" s="20"/>
+      <c r="G3" s="20"/>
+      <c r="H3" s="20"/>
+      <c r="I3" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="J3" s="21"/>
-      <c r="K3" s="21"/>
-      <c r="L3" s="21"/>
-      <c r="M3" s="21"/>
-      <c r="N3" s="21"/>
-      <c r="O3" s="21" t="s">
+      <c r="J3" s="20"/>
+      <c r="K3" s="20"/>
+      <c r="L3" s="20"/>
+      <c r="M3" s="20"/>
+      <c r="N3" s="20"/>
+      <c r="O3" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="P3" s="21"/>
-      <c r="Q3" s="21"/>
-      <c r="R3" s="21"/>
-      <c r="S3" s="21"/>
-      <c r="T3" s="21"/>
+      <c r="P3" s="20"/>
+      <c r="Q3" s="20"/>
+      <c r="R3" s="20"/>
+      <c r="S3" s="20"/>
+      <c r="T3" s="20"/>
       <c r="U3" s="15"/>
       <c r="V3" s="17"/>
       <c r="W3" s="1"/>
-      <c r="X3" s="21" t="s">
+      <c r="X3" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="Y3" s="21"/>
-      <c r="Z3" s="21"/>
-      <c r="AA3" s="21"/>
-      <c r="AB3" s="21"/>
-      <c r="AC3" s="21"/>
-      <c r="AD3" s="21" t="s">
+      <c r="Y3" s="20"/>
+      <c r="Z3" s="20"/>
+      <c r="AA3" s="20"/>
+      <c r="AB3" s="20"/>
+      <c r="AC3" s="20"/>
+      <c r="AD3" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="AE3" s="21"/>
-      <c r="AF3" s="21"/>
-      <c r="AG3" s="21"/>
-      <c r="AH3" s="21"/>
-      <c r="AI3" s="21"/>
-      <c r="AJ3" s="21" t="s">
+      <c r="AE3" s="20"/>
+      <c r="AF3" s="20"/>
+      <c r="AG3" s="20"/>
+      <c r="AH3" s="20"/>
+      <c r="AI3" s="20"/>
+      <c r="AJ3" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="AK3" s="21"/>
-      <c r="AL3" s="21"/>
-      <c r="AM3" s="21"/>
-      <c r="AN3" s="21"/>
-      <c r="AO3" s="21"/>
+      <c r="AK3" s="20"/>
+      <c r="AL3" s="20"/>
+      <c r="AM3" s="20"/>
+      <c r="AN3" s="20"/>
+      <c r="AO3" s="20"/>
     </row>
     <row r="4" spans="1:41" x14ac:dyDescent="0.25">
       <c r="C4" s="2" t="s">
@@ -806,7 +807,7 @@
       </c>
     </row>
     <row r="5" spans="1:41" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="20" t="s">
+      <c r="A5" s="21" t="s">
         <v>20</v>
       </c>
       <c r="B5" s="4" t="s">
@@ -821,14 +822,24 @@
         <f>AVERAGE(C5:G5)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="I5" s="6"/>
-      <c r="J5" s="7"/>
-      <c r="K5" s="7"/>
-      <c r="L5" s="7"/>
-      <c r="M5" s="8"/>
-      <c r="N5" s="5" t="e">
+      <c r="I5" s="6">
+        <v>0.83099999999999996</v>
+      </c>
+      <c r="J5" s="7">
+        <v>0.76400000000000001</v>
+      </c>
+      <c r="K5" s="7">
+        <v>0.753</v>
+      </c>
+      <c r="L5" s="7">
+        <v>0.76300000000000001</v>
+      </c>
+      <c r="M5" s="8">
+        <v>0.76200000000000001</v>
+      </c>
+      <c r="N5" s="5">
         <f>AVERAGE(I5:M5)</f>
-        <v>#DIV/0!</v>
+        <v>0.77459999999999996</v>
       </c>
       <c r="O5" s="6"/>
       <c r="P5" s="7"/>
@@ -840,7 +851,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="U5" s="15"/>
-      <c r="V5" s="20" t="s">
+      <c r="V5" s="21" t="s">
         <v>20</v>
       </c>
       <c r="W5" s="4" t="s">
@@ -855,14 +866,24 @@
         <f>AVERAGE(X5:AB5)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="AD5" s="6"/>
-      <c r="AE5" s="7"/>
-      <c r="AF5" s="7"/>
-      <c r="AG5" s="7"/>
-      <c r="AH5" s="8"/>
-      <c r="AI5" s="5" t="e">
+      <c r="AD5" s="6">
+        <v>35.76</v>
+      </c>
+      <c r="AE5" s="7">
+        <v>38.86</v>
+      </c>
+      <c r="AF5" s="7">
+        <v>39.44</v>
+      </c>
+      <c r="AG5" s="7">
+        <v>38.950000000000003</v>
+      </c>
+      <c r="AH5" s="8">
+        <v>38.96</v>
+      </c>
+      <c r="AI5" s="5">
         <f>AVERAGE(AD5:AH5)</f>
-        <v>#DIV/0!</v>
+        <v>38.393999999999998</v>
       </c>
       <c r="AJ5" s="6"/>
       <c r="AK5" s="7"/>
@@ -875,7 +896,7 @@
       </c>
     </row>
     <row r="6" spans="1:41" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="20"/>
+      <c r="A6" s="21"/>
       <c r="B6" s="4" t="s">
         <v>2</v>
       </c>
@@ -891,13 +912,21 @@
       <c r="I6" s="9">
         <v>118.693</v>
       </c>
-      <c r="J6" s="10"/>
-      <c r="K6" s="10"/>
-      <c r="L6" s="10"/>
-      <c r="M6" s="11"/>
+      <c r="J6" s="10">
+        <v>118.84399999999999</v>
+      </c>
+      <c r="K6" s="10">
+        <v>119.179</v>
+      </c>
+      <c r="L6" s="19">
+        <v>119.136</v>
+      </c>
+      <c r="M6" s="11">
+        <v>119.008</v>
+      </c>
       <c r="N6" s="5">
         <f t="shared" ref="N6:N13" si="1">AVERAGE(I6:M6)</f>
-        <v>118.693</v>
+        <v>118.97200000000001</v>
       </c>
       <c r="O6" s="9"/>
       <c r="P6" s="10"/>
@@ -909,7 +938,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="U6" s="15"/>
-      <c r="V6" s="20"/>
+      <c r="V6" s="21"/>
       <c r="W6" s="4" t="s">
         <v>2</v>
       </c>
@@ -925,13 +954,21 @@
       <c r="AD6" s="9">
         <v>49.54</v>
       </c>
-      <c r="AE6" s="10"/>
-      <c r="AF6" s="10"/>
-      <c r="AG6" s="10"/>
-      <c r="AH6" s="11"/>
+      <c r="AE6" s="10">
+        <v>49.48</v>
+      </c>
+      <c r="AF6" s="10">
+        <v>49.34</v>
+      </c>
+      <c r="AG6" s="19">
+        <v>49.36</v>
+      </c>
+      <c r="AH6" s="11">
+        <v>49.41</v>
+      </c>
       <c r="AI6" s="5">
         <f t="shared" ref="AI6:AI13" si="4">AVERAGE(AD6:AH6)</f>
-        <v>49.54</v>
+        <v>49.426000000000002</v>
       </c>
       <c r="AJ6" s="9"/>
       <c r="AK6" s="10"/>
@@ -944,7 +981,7 @@
       </c>
     </row>
     <row r="7" spans="1:41" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="20"/>
+      <c r="A7" s="21"/>
       <c r="B7" s="4" t="s">
         <v>3</v>
       </c>
@@ -960,13 +997,21 @@
       <c r="I7" s="9">
         <v>464.947</v>
       </c>
-      <c r="J7" s="10"/>
-      <c r="K7" s="10"/>
-      <c r="L7" s="10"/>
-      <c r="M7" s="11"/>
+      <c r="J7" s="10">
+        <v>465.71199999999999</v>
+      </c>
+      <c r="K7" s="10">
+        <v>467.06900000000002</v>
+      </c>
+      <c r="L7" s="19">
+        <v>467.01</v>
+      </c>
+      <c r="M7" s="11">
+        <v>466.88400000000001</v>
+      </c>
       <c r="N7" s="5">
         <f t="shared" si="1"/>
-        <v>464.947</v>
+        <v>466.32440000000008</v>
       </c>
       <c r="O7" s="9"/>
       <c r="P7" s="10"/>
@@ -978,7 +1023,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="U7" s="15"/>
-      <c r="V7" s="20"/>
+      <c r="V7" s="21"/>
       <c r="W7" s="4" t="s">
         <v>3</v>
       </c>
@@ -994,13 +1039,21 @@
       <c r="AD7" s="9">
         <v>44.88</v>
       </c>
-      <c r="AE7" s="10"/>
-      <c r="AF7" s="10"/>
-      <c r="AG7" s="10"/>
-      <c r="AH7" s="10"/>
+      <c r="AE7" s="10">
+        <v>44.81</v>
+      </c>
+      <c r="AF7" s="10">
+        <v>44.68</v>
+      </c>
+      <c r="AG7" s="19">
+        <v>44.68</v>
+      </c>
+      <c r="AH7" s="19">
+        <v>44.69</v>
+      </c>
       <c r="AI7" s="5">
         <f t="shared" si="4"/>
-        <v>44.88</v>
+        <v>44.748000000000005</v>
       </c>
       <c r="AJ7" s="9"/>
       <c r="AK7" s="10"/>
@@ -1013,7 +1066,7 @@
       </c>
     </row>
     <row r="8" spans="1:41" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="20"/>
+      <c r="A8" s="21"/>
       <c r="B8" s="4" t="s">
         <v>4</v>
       </c>
@@ -1047,7 +1100,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="U8" s="15"/>
-      <c r="V8" s="20"/>
+      <c r="V8" s="21"/>
       <c r="W8" s="4" t="s">
         <v>4</v>
       </c>
@@ -1082,7 +1135,7 @@
       </c>
     </row>
     <row r="9" spans="1:41" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="20"/>
+      <c r="A9" s="21"/>
       <c r="B9" s="4" t="s">
         <v>5</v>
       </c>
@@ -1116,7 +1169,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="U9" s="15"/>
-      <c r="V9" s="20"/>
+      <c r="V9" s="21"/>
       <c r="W9" s="4" t="s">
         <v>5</v>
       </c>
@@ -1159,7 +1212,7 @@
       </c>
     </row>
     <row r="10" spans="1:41" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="20"/>
+      <c r="A10" s="21"/>
       <c r="B10" s="4" t="s">
         <v>6</v>
       </c>
@@ -1172,14 +1225,24 @@
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="I10" s="9"/>
-      <c r="J10" s="10"/>
-      <c r="K10" s="10"/>
-      <c r="L10" s="10"/>
-      <c r="M10" s="11"/>
-      <c r="N10" s="5" t="e">
+      <c r="I10" s="9">
+        <v>0.33700000000000002</v>
+      </c>
+      <c r="J10" s="10">
+        <v>0.35699999999999998</v>
+      </c>
+      <c r="K10" s="10">
+        <v>0.35399999999999998</v>
+      </c>
+      <c r="L10" s="19">
+        <v>0.36099999999999999</v>
+      </c>
+      <c r="M10" s="11">
+        <v>0.34499999999999997</v>
+      </c>
+      <c r="N10" s="5">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+        <v>0.3508</v>
       </c>
       <c r="O10" s="9"/>
       <c r="P10" s="10"/>
@@ -1191,7 +1254,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="U10" s="15"/>
-      <c r="V10" s="20"/>
+      <c r="V10" s="21"/>
       <c r="W10" s="4" t="s">
         <v>6</v>
       </c>
@@ -1204,14 +1267,24 @@
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="AD10" s="9"/>
-      <c r="AE10" s="10"/>
-      <c r="AF10" s="10"/>
-      <c r="AG10" s="10"/>
-      <c r="AH10" s="11"/>
-      <c r="AI10" s="5" t="e">
+      <c r="AD10" s="9">
+        <v>662.1</v>
+      </c>
+      <c r="AE10" s="10">
+        <v>700.1</v>
+      </c>
+      <c r="AF10" s="10">
+        <v>706.5</v>
+      </c>
+      <c r="AG10" s="19">
+        <v>692</v>
+      </c>
+      <c r="AH10" s="11">
+        <v>724</v>
+      </c>
+      <c r="AI10" s="5">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
+        <v>696.93999999999994</v>
       </c>
       <c r="AJ10" s="9"/>
       <c r="AK10" s="10"/>
@@ -1224,7 +1297,7 @@
       </c>
     </row>
     <row r="11" spans="1:41" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="20"/>
+      <c r="A11" s="21"/>
       <c r="B11" s="4" t="s">
         <v>7</v>
       </c>
@@ -1237,14 +1310,24 @@
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="I11" s="9"/>
-      <c r="J11" s="10"/>
-      <c r="K11" s="10"/>
-      <c r="L11" s="10"/>
-      <c r="M11" s="11"/>
-      <c r="N11" s="5" t="e">
+      <c r="I11" s="9">
+        <v>0.38100000000000001</v>
+      </c>
+      <c r="J11" s="10">
+        <v>0.32800000000000001</v>
+      </c>
+      <c r="K11" s="10">
+        <v>0.36699999999999999</v>
+      </c>
+      <c r="L11" s="19">
+        <v>0.35399999999999998</v>
+      </c>
+      <c r="M11" s="11">
+        <v>0.36599999999999999</v>
+      </c>
+      <c r="N11" s="5">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+        <v>0.35920000000000007</v>
       </c>
       <c r="O11" s="9"/>
       <c r="P11" s="10"/>
@@ -1256,7 +1339,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="U11" s="15"/>
-      <c r="V11" s="20"/>
+      <c r="V11" s="21"/>
       <c r="W11" s="4" t="s">
         <v>7</v>
       </c>
@@ -1269,14 +1352,24 @@
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="AD11" s="9"/>
-      <c r="AE11" s="10"/>
-      <c r="AF11" s="10"/>
-      <c r="AG11" s="10"/>
-      <c r="AH11" s="11"/>
-      <c r="AI11" s="5" t="e">
+      <c r="AD11" s="9">
+        <v>1313</v>
+      </c>
+      <c r="AE11" s="10">
+        <v>1522</v>
+      </c>
+      <c r="AF11" s="10">
+        <v>1360</v>
+      </c>
+      <c r="AG11" s="19">
+        <v>1412</v>
+      </c>
+      <c r="AH11" s="11">
+        <v>1367</v>
+      </c>
+      <c r="AI11" s="5">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
+        <v>1394.8</v>
       </c>
       <c r="AJ11" s="9"/>
       <c r="AK11" s="10"/>
@@ -1289,7 +1382,7 @@
       </c>
     </row>
     <row r="12" spans="1:41" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="20"/>
+      <c r="A12" s="21"/>
       <c r="B12" s="4" t="s">
         <v>8</v>
       </c>
@@ -1302,14 +1395,24 @@
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="I12" s="9"/>
-      <c r="J12" s="10"/>
-      <c r="K12" s="10"/>
-      <c r="L12" s="10"/>
-      <c r="M12" s="11"/>
-      <c r="N12" s="5" t="e">
+      <c r="I12" s="9">
+        <v>0.38600000000000001</v>
+      </c>
+      <c r="J12" s="10">
+        <v>0.36699999999999999</v>
+      </c>
+      <c r="K12" s="10">
+        <v>0.36399999999999999</v>
+      </c>
+      <c r="L12" s="19">
+        <v>0.34899999999999998</v>
+      </c>
+      <c r="M12" s="11">
+        <v>0.36799999999999999</v>
+      </c>
+      <c r="N12" s="5">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+        <v>0.36680000000000001</v>
       </c>
       <c r="O12" s="9"/>
       <c r="P12" s="10"/>
@@ -1321,7 +1424,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="U12" s="15"/>
-      <c r="V12" s="20"/>
+      <c r="V12" s="21"/>
       <c r="W12" s="4" t="s">
         <v>8</v>
       </c>
@@ -1334,14 +1437,24 @@
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="AD12" s="9"/>
-      <c r="AE12" s="10"/>
-      <c r="AF12" s="10"/>
-      <c r="AG12" s="10"/>
-      <c r="AH12" s="11"/>
-      <c r="AI12" s="5" t="e">
+      <c r="AD12" s="9">
+        <v>1943</v>
+      </c>
+      <c r="AE12" s="10">
+        <v>2044</v>
+      </c>
+      <c r="AF12" s="10">
+        <v>2061</v>
+      </c>
+      <c r="AG12" s="19">
+        <v>2147</v>
+      </c>
+      <c r="AH12" s="11">
+        <v>2037</v>
+      </c>
+      <c r="AI12" s="5">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
+        <v>2046.4</v>
       </c>
       <c r="AJ12" s="9"/>
       <c r="AK12" s="10"/>
@@ -1354,7 +1467,7 @@
       </c>
     </row>
     <row r="13" spans="1:41" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="20"/>
+      <c r="A13" s="21"/>
       <c r="B13" s="4" t="s">
         <v>9</v>
       </c>
@@ -1367,14 +1480,24 @@
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="I13" s="12"/>
-      <c r="J13" s="13"/>
-      <c r="K13" s="13"/>
-      <c r="L13" s="13"/>
-      <c r="M13" s="14"/>
-      <c r="N13" s="5" t="e">
+      <c r="I13" s="12">
+        <v>0.38900000000000001</v>
+      </c>
+      <c r="J13" s="13">
+        <v>0.35399999999999998</v>
+      </c>
+      <c r="K13" s="13">
+        <v>0.36899999999999999</v>
+      </c>
+      <c r="L13" s="13">
+        <v>0.372</v>
+      </c>
+      <c r="M13" s="14">
+        <v>0.372</v>
+      </c>
+      <c r="N13" s="5">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+        <v>0.37119999999999997</v>
       </c>
       <c r="O13" s="12"/>
       <c r="P13" s="13"/>
@@ -1386,7 +1509,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="U13" s="15"/>
-      <c r="V13" s="20"/>
+      <c r="V13" s="21"/>
       <c r="W13" s="4" t="s">
         <v>9</v>
       </c>
@@ -1399,14 +1522,24 @@
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="AD13" s="12"/>
-      <c r="AE13" s="13"/>
-      <c r="AF13" s="13"/>
-      <c r="AG13" s="13"/>
-      <c r="AH13" s="14"/>
-      <c r="AI13" s="5" t="e">
+      <c r="AD13" s="12">
+        <v>2569</v>
+      </c>
+      <c r="AE13" s="13">
+        <v>2819</v>
+      </c>
+      <c r="AF13" s="13">
+        <v>2706</v>
+      </c>
+      <c r="AG13" s="13">
+        <v>2685</v>
+      </c>
+      <c r="AH13" s="14">
+        <v>2683</v>
+      </c>
+      <c r="AI13" s="5">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
+        <v>2692.4</v>
       </c>
       <c r="AJ13" s="12"/>
       <c r="AK13" s="13"/>
@@ -1462,7 +1595,7 @@
       <c r="AO14" s="15"/>
     </row>
     <row r="15" spans="1:41" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="20" t="s">
+      <c r="A15" s="21" t="s">
         <v>21</v>
       </c>
       <c r="B15" s="4" t="s">
@@ -1477,14 +1610,24 @@
         <f>AVERAGE(C15:G15)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="I15" s="6"/>
-      <c r="J15" s="7"/>
-      <c r="K15" s="7"/>
-      <c r="L15" s="7"/>
-      <c r="M15" s="8"/>
-      <c r="N15" s="5" t="e">
+      <c r="I15" s="6">
+        <v>0.752</v>
+      </c>
+      <c r="J15" s="7">
+        <v>0.69499999999999995</v>
+      </c>
+      <c r="K15" s="7">
+        <v>0.70099999999999996</v>
+      </c>
+      <c r="L15" s="7">
+        <v>0.69699999999999995</v>
+      </c>
+      <c r="M15" s="8">
+        <v>0.70599999999999996</v>
+      </c>
+      <c r="N15" s="5">
         <f>AVERAGE(I15:M15)</f>
-        <v>#DIV/0!</v>
+        <v>0.71020000000000005</v>
       </c>
       <c r="O15" s="6"/>
       <c r="P15" s="7"/>
@@ -1496,7 +1639,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="U15" s="15"/>
-      <c r="V15" s="20" t="s">
+      <c r="V15" s="21" t="s">
         <v>21</v>
       </c>
       <c r="W15" s="4" t="s">
@@ -1511,14 +1654,24 @@
         <f>AVERAGE(X15:AB15)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="AD15" s="6"/>
-      <c r="AE15" s="7"/>
-      <c r="AF15" s="7"/>
-      <c r="AG15" s="7"/>
-      <c r="AH15" s="8"/>
-      <c r="AI15" s="5" t="e">
+      <c r="AD15" s="6">
+        <v>39.49</v>
+      </c>
+      <c r="AE15" s="7">
+        <v>42.73</v>
+      </c>
+      <c r="AF15" s="7">
+        <v>42.39</v>
+      </c>
+      <c r="AG15" s="7">
+        <v>42.59</v>
+      </c>
+      <c r="AH15" s="8">
+        <v>42.08</v>
+      </c>
+      <c r="AI15" s="5">
         <f>AVERAGE(AD15:AH15)</f>
-        <v>#DIV/0!</v>
+        <v>41.855999999999995</v>
       </c>
       <c r="AJ15" s="6"/>
       <c r="AK15" s="7"/>
@@ -1531,7 +1684,7 @@
       </c>
     </row>
     <row r="16" spans="1:41" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="20"/>
+      <c r="A16" s="21"/>
       <c r="B16" s="4" t="s">
         <v>2</v>
       </c>
@@ -1547,13 +1700,21 @@
       <c r="I16" s="9">
         <v>101.76300000000001</v>
       </c>
-      <c r="J16" s="10"/>
-      <c r="K16" s="10"/>
-      <c r="L16" s="10"/>
-      <c r="M16" s="11"/>
+      <c r="J16" s="19">
+        <v>101.23399999999999</v>
+      </c>
+      <c r="K16" s="19">
+        <v>101.715</v>
+      </c>
+      <c r="L16" s="19">
+        <v>101.655</v>
+      </c>
+      <c r="M16" s="11">
+        <v>101.577</v>
+      </c>
       <c r="N16" s="5">
         <f t="shared" ref="N16:N23" si="7">AVERAGE(I16:M16)</f>
-        <v>101.76300000000001</v>
+        <v>101.58879999999999</v>
       </c>
       <c r="O16" s="9"/>
       <c r="P16" s="10"/>
@@ -1565,7 +1726,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="U16" s="15"/>
-      <c r="V16" s="20"/>
+      <c r="V16" s="21"/>
       <c r="W16" s="4" t="s">
         <v>2</v>
       </c>
@@ -1581,13 +1742,21 @@
       <c r="AD16" s="9">
         <v>57.79</v>
       </c>
-      <c r="AE16" s="10"/>
-      <c r="AF16" s="10"/>
-      <c r="AG16" s="10"/>
-      <c r="AH16" s="11"/>
+      <c r="AE16" s="19">
+        <v>58.09</v>
+      </c>
+      <c r="AF16" s="19">
+        <v>57.81</v>
+      </c>
+      <c r="AG16" s="19">
+        <v>57.85</v>
+      </c>
+      <c r="AH16" s="11">
+        <v>57.89</v>
+      </c>
       <c r="AI16" s="5">
-        <f t="shared" ref="AI16:AI23" si="10">AVERAGE(AD16:AH16)</f>
-        <v>57.79</v>
+        <f t="shared" ref="AI16:AI22" si="10">AVERAGE(AD16:AH16)</f>
+        <v>57.886000000000003</v>
       </c>
       <c r="AJ16" s="9"/>
       <c r="AK16" s="10"/>
@@ -1600,7 +1769,7 @@
       </c>
     </row>
     <row r="17" spans="1:41" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="20"/>
+      <c r="A17" s="21"/>
       <c r="B17" s="4" t="s">
         <v>3</v>
       </c>
@@ -1616,13 +1785,21 @@
       <c r="I17" s="9">
         <v>397.11799999999999</v>
       </c>
-      <c r="J17" s="10"/>
-      <c r="K17" s="10"/>
-      <c r="L17" s="10"/>
-      <c r="M17" s="11"/>
+      <c r="J17" s="19">
+        <v>397.935</v>
+      </c>
+      <c r="K17" s="19">
+        <v>399.476</v>
+      </c>
+      <c r="L17" s="19">
+        <v>400.22699999999998</v>
+      </c>
+      <c r="M17" s="11">
+        <v>400.31200000000001</v>
+      </c>
       <c r="N17" s="5">
         <f t="shared" si="7"/>
-        <v>397.11799999999999</v>
+        <v>399.01359999999994</v>
       </c>
       <c r="O17" s="9"/>
       <c r="P17" s="10"/>
@@ -1634,7 +1811,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="U17" s="15"/>
-      <c r="V17" s="20"/>
+      <c r="V17" s="21"/>
       <c r="W17" s="4" t="s">
         <v>3</v>
       </c>
@@ -1650,13 +1827,21 @@
       <c r="AD17" s="9">
         <v>52.55</v>
       </c>
-      <c r="AE17" s="10"/>
-      <c r="AF17" s="10"/>
-      <c r="AG17" s="10"/>
-      <c r="AH17" s="10"/>
+      <c r="AE17" s="19">
+        <v>52.44</v>
+      </c>
+      <c r="AF17" s="19">
+        <v>52.24</v>
+      </c>
+      <c r="AG17" s="19">
+        <v>52.14</v>
+      </c>
+      <c r="AH17" s="19">
+        <v>52.13</v>
+      </c>
       <c r="AI17" s="5">
         <f t="shared" si="10"/>
-        <v>52.55</v>
+        <v>52.3</v>
       </c>
       <c r="AJ17" s="9"/>
       <c r="AK17" s="10"/>
@@ -1669,7 +1854,7 @@
       </c>
     </row>
     <row r="18" spans="1:41" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="20"/>
+      <c r="A18" s="21"/>
       <c r="B18" s="4" t="s">
         <v>4</v>
       </c>
@@ -1703,7 +1888,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="U18" s="15"/>
-      <c r="V18" s="20"/>
+      <c r="V18" s="21"/>
       <c r="W18" s="4" t="s">
         <v>4</v>
       </c>
@@ -1738,7 +1923,7 @@
       </c>
     </row>
     <row r="19" spans="1:41" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="20"/>
+      <c r="A19" s="21"/>
       <c r="B19" s="4" t="s">
         <v>5</v>
       </c>
@@ -1772,7 +1957,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="U19" s="15"/>
-      <c r="V19" s="20"/>
+      <c r="V19" s="21"/>
       <c r="W19" s="4" t="s">
         <v>5</v>
       </c>
@@ -1815,7 +2000,7 @@
       </c>
     </row>
     <row r="20" spans="1:41" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="20"/>
+      <c r="A20" s="21"/>
       <c r="B20" s="4" t="s">
         <v>6</v>
       </c>
@@ -1828,14 +2013,24 @@
         <f t="shared" si="6"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="I20" s="9"/>
-      <c r="J20" s="10"/>
-      <c r="K20" s="10"/>
-      <c r="L20" s="10"/>
-      <c r="M20" s="11"/>
-      <c r="N20" s="5" t="e">
+      <c r="I20" s="9">
+        <v>0.34799999999999998</v>
+      </c>
+      <c r="J20" s="10">
+        <v>0.32900000000000001</v>
+      </c>
+      <c r="K20" s="10">
+        <v>0.35</v>
+      </c>
+      <c r="L20" s="19">
+        <v>0.34</v>
+      </c>
+      <c r="M20" s="11">
+        <v>0.34899999999999998</v>
+      </c>
+      <c r="N20" s="5">
         <f t="shared" si="7"/>
-        <v>#DIV/0!</v>
+        <v>0.34320000000000006</v>
       </c>
       <c r="O20" s="9"/>
       <c r="P20" s="10"/>
@@ -1847,7 +2042,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="U20" s="15"/>
-      <c r="V20" s="20"/>
+      <c r="V20" s="21"/>
       <c r="W20" s="4" t="s">
         <v>6</v>
       </c>
@@ -1860,14 +2055,24 @@
         <f t="shared" si="9"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="AD20" s="9"/>
-      <c r="AE20" s="10"/>
-      <c r="AF20" s="10"/>
-      <c r="AG20" s="10"/>
-      <c r="AH20" s="11"/>
-      <c r="AI20" s="5" t="e">
+      <c r="AD20" s="9">
+        <v>718.8</v>
+      </c>
+      <c r="AE20" s="10">
+        <v>759</v>
+      </c>
+      <c r="AF20" s="10">
+        <v>714.7</v>
+      </c>
+      <c r="AG20" s="19">
+        <v>735.3</v>
+      </c>
+      <c r="AH20" s="11">
+        <v>716.7</v>
+      </c>
+      <c r="AI20" s="5">
         <f t="shared" si="10"/>
-        <v>#DIV/0!</v>
+        <v>728.9</v>
       </c>
       <c r="AJ20" s="9"/>
       <c r="AK20" s="10"/>
@@ -1880,7 +2085,7 @@
       </c>
     </row>
     <row r="21" spans="1:41" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="20"/>
+      <c r="A21" s="21"/>
       <c r="B21" s="4" t="s">
         <v>7</v>
       </c>
@@ -1893,14 +2098,24 @@
         <f t="shared" si="6"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="I21" s="9"/>
-      <c r="J21" s="10"/>
-      <c r="K21" s="10"/>
-      <c r="L21" s="10"/>
-      <c r="M21" s="11"/>
-      <c r="N21" s="5" t="e">
+      <c r="I21" s="9">
+        <v>0.38</v>
+      </c>
+      <c r="J21" s="10">
+        <v>0.34200000000000003</v>
+      </c>
+      <c r="K21" s="10">
+        <v>0.35499999999999998</v>
+      </c>
+      <c r="L21" s="19">
+        <v>0.36499999999999999</v>
+      </c>
+      <c r="M21" s="11">
+        <v>0.35899999999999999</v>
+      </c>
+      <c r="N21" s="5">
         <f t="shared" si="7"/>
-        <v>#DIV/0!</v>
+        <v>0.36019999999999996</v>
       </c>
       <c r="O21" s="9"/>
       <c r="P21" s="10"/>
@@ -1912,7 +2127,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="U21" s="15"/>
-      <c r="V21" s="20"/>
+      <c r="V21" s="21"/>
       <c r="W21" s="4" t="s">
         <v>7</v>
       </c>
@@ -1925,14 +2140,24 @@
         <f t="shared" si="9"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="AD21" s="9"/>
-      <c r="AE21" s="10"/>
-      <c r="AF21" s="10"/>
-      <c r="AG21" s="10"/>
-      <c r="AH21" s="11"/>
-      <c r="AI21" s="5" t="e">
+      <c r="AD21" s="9">
+        <v>1313</v>
+      </c>
+      <c r="AE21" s="10">
+        <v>1462</v>
+      </c>
+      <c r="AF21" s="10">
+        <v>1408</v>
+      </c>
+      <c r="AG21" s="19">
+        <v>1370</v>
+      </c>
+      <c r="AH21" s="11">
+        <v>1392</v>
+      </c>
+      <c r="AI21" s="5">
         <f t="shared" si="10"/>
-        <v>#DIV/0!</v>
+        <v>1389</v>
       </c>
       <c r="AJ21" s="9"/>
       <c r="AK21" s="10"/>
@@ -1945,7 +2170,7 @@
       </c>
     </row>
     <row r="22" spans="1:41" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="20"/>
+      <c r="A22" s="21"/>
       <c r="B22" s="4" t="s">
         <v>8</v>
       </c>
@@ -1958,14 +2183,24 @@
         <f t="shared" si="6"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="I22" s="9"/>
-      <c r="J22" s="10"/>
-      <c r="K22" s="10"/>
-      <c r="L22" s="10"/>
-      <c r="M22" s="11"/>
-      <c r="N22" s="5" t="e">
+      <c r="I22" s="9">
+        <v>0.38100000000000001</v>
+      </c>
+      <c r="J22" s="10">
+        <v>0.36699999999999999</v>
+      </c>
+      <c r="K22" s="10">
+        <v>0.36499999999999999</v>
+      </c>
+      <c r="L22" s="19">
+        <v>0.35299999999999998</v>
+      </c>
+      <c r="M22" s="11">
+        <v>0.35699999999999998</v>
+      </c>
+      <c r="N22" s="5">
         <f t="shared" si="7"/>
-        <v>#DIV/0!</v>
+        <v>0.36459999999999998</v>
       </c>
       <c r="O22" s="9"/>
       <c r="P22" s="10"/>
@@ -1977,7 +2212,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="U22" s="15"/>
-      <c r="V22" s="20"/>
+      <c r="V22" s="21"/>
       <c r="W22" s="4" t="s">
         <v>8</v>
       </c>
@@ -1990,14 +2225,24 @@
         <f t="shared" si="9"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="AD22" s="9"/>
-      <c r="AE22" s="10"/>
-      <c r="AF22" s="10"/>
-      <c r="AG22" s="10"/>
-      <c r="AH22" s="11"/>
-      <c r="AI22" s="5" t="e">
+      <c r="AD22" s="9">
+        <v>1969</v>
+      </c>
+      <c r="AE22" s="10">
+        <v>2041</v>
+      </c>
+      <c r="AF22" s="10">
+        <v>2055</v>
+      </c>
+      <c r="AG22" s="19">
+        <v>2125</v>
+      </c>
+      <c r="AH22" s="11">
+        <v>2100</v>
+      </c>
+      <c r="AI22" s="5">
         <f t="shared" si="10"/>
-        <v>#DIV/0!</v>
+        <v>2058</v>
       </c>
       <c r="AJ22" s="9"/>
       <c r="AK22" s="10"/>
@@ -2010,7 +2255,7 @@
       </c>
     </row>
     <row r="23" spans="1:41" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="20"/>
+      <c r="A23" s="21"/>
       <c r="B23" s="4" t="s">
         <v>9</v>
       </c>
@@ -2023,14 +2268,24 @@
         <f t="shared" si="6"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="I23" s="12"/>
-      <c r="J23" s="13"/>
-      <c r="K23" s="13"/>
-      <c r="L23" s="13"/>
-      <c r="M23" s="14"/>
-      <c r="N23" s="5" t="e">
+      <c r="I23" s="12">
+        <v>0.34899999999999998</v>
+      </c>
+      <c r="J23" s="13">
+        <v>0.34200000000000003</v>
+      </c>
+      <c r="K23" s="13">
+        <v>0.373</v>
+      </c>
+      <c r="L23" s="13">
+        <v>0.36099999999999999</v>
+      </c>
+      <c r="M23" s="14">
+        <v>0.34300000000000003</v>
+      </c>
+      <c r="N23" s="5">
         <f t="shared" si="7"/>
-        <v>#DIV/0!</v>
+        <v>0.35360000000000003</v>
       </c>
       <c r="O23" s="12"/>
       <c r="P23" s="13"/>
@@ -2042,7 +2297,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="U23" s="15"/>
-      <c r="V23" s="20"/>
+      <c r="V23" s="21"/>
       <c r="W23" s="4" t="s">
         <v>9</v>
       </c>
@@ -2055,14 +2310,24 @@
         <f t="shared" si="9"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="AD23" s="12"/>
-      <c r="AE23" s="13"/>
-      <c r="AF23" s="13"/>
-      <c r="AG23" s="13"/>
-      <c r="AH23" s="14"/>
-      <c r="AI23" s="5" t="e">
-        <f t="shared" si="10"/>
-        <v>#DIV/0!</v>
+      <c r="AD23" s="12">
+        <v>2861</v>
+      </c>
+      <c r="AE23" s="13">
+        <v>2918</v>
+      </c>
+      <c r="AF23" s="13">
+        <v>2675</v>
+      </c>
+      <c r="AG23" s="13">
+        <v>2764</v>
+      </c>
+      <c r="AH23" s="14">
+        <v>2911</v>
+      </c>
+      <c r="AI23" s="5">
+        <f>AVERAGE(AD23:AH23)</f>
+        <v>2825.8</v>
       </c>
       <c r="AJ23" s="12"/>
       <c r="AK23" s="13"/>
@@ -2118,7 +2383,7 @@
       <c r="AO24" s="15"/>
     </row>
     <row r="25" spans="1:41" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="20" t="s">
+      <c r="A25" s="21" t="s">
         <v>22</v>
       </c>
       <c r="B25" s="4" t="s">
@@ -2133,14 +2398,24 @@
         <f>AVERAGE(C25:G25)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="I25" s="6"/>
-      <c r="J25" s="7"/>
-      <c r="K25" s="7"/>
-      <c r="L25" s="7"/>
-      <c r="M25" s="8"/>
-      <c r="N25" s="5" t="e">
+      <c r="I25" s="6">
+        <v>0.64500000000000002</v>
+      </c>
+      <c r="J25" s="7">
+        <v>0.55500000000000005</v>
+      </c>
+      <c r="K25" s="7">
+        <v>0.58499999999999996</v>
+      </c>
+      <c r="L25" s="7">
+        <v>0.57399999999999995</v>
+      </c>
+      <c r="M25" s="8">
+        <v>0.56499999999999995</v>
+      </c>
+      <c r="N25" s="5">
         <f>AVERAGE(I25:M25)</f>
-        <v>#DIV/0!</v>
+        <v>0.58479999999999999</v>
       </c>
       <c r="O25" s="6"/>
       <c r="P25" s="7"/>
@@ -2152,7 +2427,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="U25" s="15"/>
-      <c r="V25" s="20" t="s">
+      <c r="V25" s="21" t="s">
         <v>22</v>
       </c>
       <c r="W25" s="4" t="s">
@@ -2167,14 +2442,24 @@
         <f>AVERAGE(X25:AB25)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="AD25" s="6"/>
-      <c r="AE25" s="7"/>
-      <c r="AF25" s="7"/>
-      <c r="AG25" s="7"/>
-      <c r="AH25" s="8"/>
-      <c r="AI25" s="5" t="e">
+      <c r="AD25" s="6">
+        <v>46.05</v>
+      </c>
+      <c r="AE25" s="7">
+        <v>53.54</v>
+      </c>
+      <c r="AF25" s="7">
+        <v>50.82</v>
+      </c>
+      <c r="AG25" s="7">
+        <v>51.78</v>
+      </c>
+      <c r="AH25" s="8">
+        <v>52.54</v>
+      </c>
+      <c r="AI25" s="5">
         <f>AVERAGE(AD25:AH25)</f>
-        <v>#DIV/0!</v>
+        <v>50.945999999999998</v>
       </c>
       <c r="AJ25" s="6"/>
       <c r="AK25" s="7"/>
@@ -2187,7 +2472,7 @@
       </c>
     </row>
     <row r="26" spans="1:41" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="20"/>
+      <c r="A26" s="21"/>
       <c r="B26" s="4" t="s">
         <v>2</v>
       </c>
@@ -2203,13 +2488,21 @@
       <c r="I26" s="9">
         <v>64.331999999999994</v>
       </c>
-      <c r="J26" s="10"/>
-      <c r="K26" s="10"/>
-      <c r="L26" s="10"/>
-      <c r="M26" s="11"/>
+      <c r="J26" s="19">
+        <v>64.582999999999998</v>
+      </c>
+      <c r="K26" s="19">
+        <v>64.918000000000006</v>
+      </c>
+      <c r="L26" s="19">
+        <v>64.858000000000004</v>
+      </c>
+      <c r="M26" s="11">
+        <v>64.866</v>
+      </c>
       <c r="N26" s="5">
         <f t="shared" ref="N26:N33" si="13">AVERAGE(I26:M26)</f>
-        <v>64.331999999999994</v>
+        <v>64.711399999999998</v>
       </c>
       <c r="O26" s="9"/>
       <c r="P26" s="10"/>
@@ -2221,7 +2514,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="U26" s="15"/>
-      <c r="V26" s="20"/>
+      <c r="V26" s="21"/>
       <c r="W26" s="4" t="s">
         <v>2</v>
       </c>
@@ -2237,13 +2530,21 @@
       <c r="AD26" s="9">
         <v>91.41</v>
       </c>
-      <c r="AE26" s="10"/>
-      <c r="AF26" s="10"/>
-      <c r="AG26" s="10"/>
-      <c r="AH26" s="11"/>
+      <c r="AE26" s="19">
+        <v>91.05</v>
+      </c>
+      <c r="AF26" s="19">
+        <v>90.58</v>
+      </c>
+      <c r="AG26" s="19">
+        <v>90.67</v>
+      </c>
+      <c r="AH26" s="11">
+        <v>90.66</v>
+      </c>
       <c r="AI26" s="5">
         <f t="shared" ref="AI26:AI33" si="16">AVERAGE(AD26:AH26)</f>
-        <v>91.41</v>
+        <v>90.873999999999995</v>
       </c>
       <c r="AJ26" s="9"/>
       <c r="AK26" s="10"/>
@@ -2256,7 +2557,7 @@
       </c>
     </row>
     <row r="27" spans="1:41" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="20"/>
+      <c r="A27" s="21"/>
       <c r="B27" s="4" t="s">
         <v>3</v>
       </c>
@@ -2290,7 +2591,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="U27" s="15"/>
-      <c r="V27" s="20"/>
+      <c r="V27" s="21"/>
       <c r="W27" s="4" t="s">
         <v>3</v>
       </c>
@@ -2325,7 +2626,7 @@
       </c>
     </row>
     <row r="28" spans="1:41" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="20"/>
+      <c r="A28" s="21"/>
       <c r="B28" s="4" t="s">
         <v>4</v>
       </c>
@@ -2359,7 +2660,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="U28" s="15"/>
-      <c r="V28" s="20"/>
+      <c r="V28" s="21"/>
       <c r="W28" s="4" t="s">
         <v>4</v>
       </c>
@@ -2394,7 +2695,7 @@
       </c>
     </row>
     <row r="29" spans="1:41" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="20"/>
+      <c r="A29" s="21"/>
       <c r="B29" s="4" t="s">
         <v>5</v>
       </c>
@@ -2428,7 +2729,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="U29" s="15"/>
-      <c r="V29" s="20"/>
+      <c r="V29" s="21"/>
       <c r="W29" s="4" t="s">
         <v>5</v>
       </c>
@@ -2471,7 +2772,7 @@
       </c>
     </row>
     <row r="30" spans="1:41" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="20"/>
+      <c r="A30" s="21"/>
       <c r="B30" s="4" t="s">
         <v>6</v>
       </c>
@@ -2484,14 +2785,24 @@
         <f t="shared" si="12"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="I30" s="9"/>
-      <c r="J30" s="10"/>
-      <c r="K30" s="10"/>
-      <c r="L30" s="10"/>
-      <c r="M30" s="11"/>
-      <c r="N30" s="5" t="e">
+      <c r="I30" s="9">
+        <v>0.314</v>
+      </c>
+      <c r="J30" s="10">
+        <v>0.29399999999999998</v>
+      </c>
+      <c r="K30" s="10">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="L30" s="19">
+        <v>0.29499999999999998</v>
+      </c>
+      <c r="M30" s="11">
+        <v>0.28699999999999998</v>
+      </c>
+      <c r="N30" s="5">
         <f t="shared" si="13"/>
-        <v>#DIV/0!</v>
+        <v>0.29599999999999993</v>
       </c>
       <c r="O30" s="9"/>
       <c r="P30" s="10"/>
@@ -2503,7 +2814,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="U30" s="15"/>
-      <c r="V30" s="20"/>
+      <c r="V30" s="21"/>
       <c r="W30" s="4" t="s">
         <v>6</v>
       </c>
@@ -2516,14 +2827,24 @@
         <f t="shared" si="15"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="AD30" s="9"/>
-      <c r="AE30" s="10"/>
-      <c r="AF30" s="10"/>
-      <c r="AG30" s="10"/>
-      <c r="AH30" s="11"/>
-      <c r="AI30" s="5" t="e">
+      <c r="AD30" s="9">
+        <v>796.8</v>
+      </c>
+      <c r="AE30" s="10">
+        <v>850.6</v>
+      </c>
+      <c r="AF30" s="10">
+        <v>861</v>
+      </c>
+      <c r="AG30" s="19">
+        <v>847.1</v>
+      </c>
+      <c r="AH30" s="11">
+        <v>871.6</v>
+      </c>
+      <c r="AI30" s="5">
         <f t="shared" si="16"/>
-        <v>#DIV/0!</v>
+        <v>845.42000000000007</v>
       </c>
       <c r="AJ30" s="9"/>
       <c r="AK30" s="10"/>
@@ -2536,7 +2857,7 @@
       </c>
     </row>
     <row r="31" spans="1:41" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="20"/>
+      <c r="A31" s="21"/>
       <c r="B31" s="4" t="s">
         <v>7</v>
       </c>
@@ -2549,14 +2870,24 @@
         <f t="shared" si="12"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="I31" s="9"/>
-      <c r="J31" s="10"/>
-      <c r="K31" s="10"/>
-      <c r="L31" s="10"/>
-      <c r="M31" s="11"/>
-      <c r="N31" s="5" t="e">
+      <c r="I31" s="9">
+        <v>0.311</v>
+      </c>
+      <c r="J31" s="10">
+        <v>0.316</v>
+      </c>
+      <c r="K31" s="10">
+        <v>0.312</v>
+      </c>
+      <c r="L31" s="19">
+        <v>0.315</v>
+      </c>
+      <c r="M31" s="11">
+        <v>0.317</v>
+      </c>
+      <c r="N31" s="5">
         <f t="shared" si="13"/>
-        <v>#DIV/0!</v>
+        <v>0.31419999999999998</v>
       </c>
       <c r="O31" s="9"/>
       <c r="P31" s="10"/>
@@ -2568,7 +2899,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="U31" s="15"/>
-      <c r="V31" s="20"/>
+      <c r="V31" s="21"/>
       <c r="W31" s="4" t="s">
         <v>7</v>
       </c>
@@ -2581,14 +2912,24 @@
         <f t="shared" si="15"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="AD31" s="9"/>
-      <c r="AE31" s="10"/>
-      <c r="AF31" s="10"/>
-      <c r="AG31" s="10"/>
-      <c r="AH31" s="11"/>
-      <c r="AI31" s="5" t="e">
+      <c r="AD31" s="9">
+        <v>1605</v>
+      </c>
+      <c r="AE31" s="10">
+        <v>1580</v>
+      </c>
+      <c r="AF31" s="10">
+        <v>1600</v>
+      </c>
+      <c r="AG31" s="19">
+        <v>1587</v>
+      </c>
+      <c r="AH31" s="11">
+        <v>1575</v>
+      </c>
+      <c r="AI31" s="5">
         <f t="shared" si="16"/>
-        <v>#DIV/0!</v>
+        <v>1589.4</v>
       </c>
       <c r="AJ31" s="9"/>
       <c r="AK31" s="10"/>
@@ -2601,7 +2942,7 @@
       </c>
     </row>
     <row r="32" spans="1:41" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="20"/>
+      <c r="A32" s="21"/>
       <c r="B32" s="4" t="s">
         <v>8</v>
       </c>
@@ -2614,14 +2955,24 @@
         <f t="shared" si="12"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="I32" s="9"/>
-      <c r="J32" s="10"/>
-      <c r="K32" s="10"/>
-      <c r="L32" s="10"/>
-      <c r="M32" s="11"/>
-      <c r="N32" s="5" t="e">
+      <c r="I32" s="9">
+        <v>0.33200000000000002</v>
+      </c>
+      <c r="J32" s="10">
+        <v>0.308</v>
+      </c>
+      <c r="K32" s="10">
+        <v>0.32</v>
+      </c>
+      <c r="L32" s="19">
+        <v>0.32200000000000001</v>
+      </c>
+      <c r="M32" s="11">
+        <v>0.32</v>
+      </c>
+      <c r="N32" s="5">
         <f t="shared" si="13"/>
-        <v>#DIV/0!</v>
+        <v>0.32040000000000002</v>
       </c>
       <c r="O32" s="9"/>
       <c r="P32" s="10"/>
@@ -2633,7 +2984,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="U32" s="15"/>
-      <c r="V32" s="20"/>
+      <c r="V32" s="21"/>
       <c r="W32" s="4" t="s">
         <v>8</v>
       </c>
@@ -2646,14 +2997,24 @@
         <f t="shared" si="15"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="AD32" s="9"/>
-      <c r="AE32" s="10"/>
-      <c r="AF32" s="10"/>
-      <c r="AG32" s="10"/>
-      <c r="AH32" s="11"/>
-      <c r="AI32" s="5" t="e">
+      <c r="AD32" s="9">
+        <v>2258</v>
+      </c>
+      <c r="AE32" s="10">
+        <v>2433</v>
+      </c>
+      <c r="AF32" s="10">
+        <v>2344</v>
+      </c>
+      <c r="AG32" s="19">
+        <v>2327</v>
+      </c>
+      <c r="AH32" s="11">
+        <v>2342</v>
+      </c>
+      <c r="AI32" s="5">
         <f t="shared" si="16"/>
-        <v>#DIV/0!</v>
+        <v>2340.8000000000002</v>
       </c>
       <c r="AJ32" s="9"/>
       <c r="AK32" s="10"/>
@@ -2666,7 +3027,7 @@
       </c>
     </row>
     <row r="33" spans="1:41" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="20"/>
+      <c r="A33" s="21"/>
       <c r="B33" s="4" t="s">
         <v>9</v>
       </c>
@@ -2679,14 +3040,24 @@
         <f t="shared" si="12"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="I33" s="12"/>
-      <c r="J33" s="13"/>
-      <c r="K33" s="13"/>
-      <c r="L33" s="13"/>
-      <c r="M33" s="14"/>
-      <c r="N33" s="5" t="e">
+      <c r="I33" s="12">
+        <v>0.34200000000000003</v>
+      </c>
+      <c r="J33" s="13">
+        <v>0.29499999999999998</v>
+      </c>
+      <c r="K33" s="13">
+        <v>0.31900000000000001</v>
+      </c>
+      <c r="L33" s="13">
+        <v>0.316</v>
+      </c>
+      <c r="M33" s="14">
+        <v>0.32500000000000001</v>
+      </c>
+      <c r="N33" s="5">
         <f t="shared" si="13"/>
-        <v>#DIV/0!</v>
+        <v>0.31940000000000002</v>
       </c>
       <c r="O33" s="12"/>
       <c r="P33" s="13"/>
@@ -2698,7 +3069,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="U33" s="15"/>
-      <c r="V33" s="20"/>
+      <c r="V33" s="21"/>
       <c r="W33" s="4" t="s">
         <v>9</v>
       </c>
@@ -2711,14 +3082,24 @@
         <f t="shared" si="15"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="AD33" s="12"/>
-      <c r="AE33" s="13"/>
-      <c r="AF33" s="13"/>
-      <c r="AG33" s="13"/>
-      <c r="AH33" s="14"/>
-      <c r="AI33" s="5" t="e">
+      <c r="AD33" s="12">
+        <v>2920</v>
+      </c>
+      <c r="AE33" s="13">
+        <v>3386</v>
+      </c>
+      <c r="AF33" s="13">
+        <v>3134</v>
+      </c>
+      <c r="AG33" s="13">
+        <v>3164</v>
+      </c>
+      <c r="AH33" s="14">
+        <v>3078</v>
+      </c>
+      <c r="AI33" s="5">
         <f t="shared" si="16"/>
-        <v>#DIV/0!</v>
+        <v>3136.4</v>
       </c>
       <c r="AJ33" s="12"/>
       <c r="AK33" s="13"/>
@@ -2774,7 +3155,7 @@
       <c r="AO34" s="15"/>
     </row>
     <row r="35" spans="1:41" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="20" t="s">
+      <c r="A35" s="21" t="s">
         <v>23</v>
       </c>
       <c r="B35" s="4" t="s">
@@ -2808,7 +3189,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="U35" s="15"/>
-      <c r="V35" s="20" t="s">
+      <c r="V35" s="21" t="s">
         <v>23</v>
       </c>
       <c r="W35" s="4" t="s">
@@ -2843,7 +3224,7 @@
       </c>
     </row>
     <row r="36" spans="1:41" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="20"/>
+      <c r="A36" s="21"/>
       <c r="B36" s="4" t="s">
         <v>2</v>
       </c>
@@ -2875,7 +3256,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="U36" s="15"/>
-      <c r="V36" s="20"/>
+      <c r="V36" s="21"/>
       <c r="W36" s="4" t="s">
         <v>2</v>
       </c>
@@ -2908,7 +3289,7 @@
       </c>
     </row>
     <row r="37" spans="1:41" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="20"/>
+      <c r="A37" s="21"/>
       <c r="B37" s="4" t="s">
         <v>3</v>
       </c>
@@ -2940,7 +3321,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="U37" s="15"/>
-      <c r="V37" s="20"/>
+      <c r="V37" s="21"/>
       <c r="W37" s="4" t="s">
         <v>3</v>
       </c>
@@ -2973,7 +3354,7 @@
       </c>
     </row>
     <row r="38" spans="1:41" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="20"/>
+      <c r="A38" s="21"/>
       <c r="B38" s="4" t="s">
         <v>4</v>
       </c>
@@ -3005,7 +3386,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="U38" s="15"/>
-      <c r="V38" s="20"/>
+      <c r="V38" s="21"/>
       <c r="W38" s="4" t="s">
         <v>4</v>
       </c>
@@ -3038,7 +3419,7 @@
       </c>
     </row>
     <row r="39" spans="1:41" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="20"/>
+      <c r="A39" s="21"/>
       <c r="B39" s="4" t="s">
         <v>5</v>
       </c>
@@ -3070,7 +3451,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="U39" s="15"/>
-      <c r="V39" s="20"/>
+      <c r="V39" s="21"/>
       <c r="W39" s="4" t="s">
         <v>5</v>
       </c>
@@ -3103,7 +3484,7 @@
       </c>
     </row>
     <row r="40" spans="1:41" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="20"/>
+      <c r="A40" s="21"/>
       <c r="B40" s="4" t="s">
         <v>6</v>
       </c>
@@ -3135,7 +3516,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="U40" s="15"/>
-      <c r="V40" s="20"/>
+      <c r="V40" s="21"/>
       <c r="W40" s="4" t="s">
         <v>6</v>
       </c>
@@ -3168,7 +3549,7 @@
       </c>
     </row>
     <row r="41" spans="1:41" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="20"/>
+      <c r="A41" s="21"/>
       <c r="B41" s="4" t="s">
         <v>7</v>
       </c>
@@ -3200,7 +3581,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="U41" s="15"/>
-      <c r="V41" s="20"/>
+      <c r="V41" s="21"/>
       <c r="W41" s="4" t="s">
         <v>7</v>
       </c>
@@ -3233,7 +3614,7 @@
       </c>
     </row>
     <row r="42" spans="1:41" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="20"/>
+      <c r="A42" s="21"/>
       <c r="B42" s="4" t="s">
         <v>8</v>
       </c>
@@ -3265,7 +3646,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="U42" s="15"/>
-      <c r="V42" s="20"/>
+      <c r="V42" s="21"/>
       <c r="W42" s="4" t="s">
         <v>8</v>
       </c>
@@ -3298,7 +3679,7 @@
       </c>
     </row>
     <row r="43" spans="1:41" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="20"/>
+      <c r="A43" s="21"/>
       <c r="B43" s="4" t="s">
         <v>9</v>
       </c>
@@ -3330,7 +3711,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="U43" s="15"/>
-      <c r="V43" s="20"/>
+      <c r="V43" s="21"/>
       <c r="W43" s="4" t="s">
         <v>9</v>
       </c>
@@ -3524,6 +3905,12 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="A1:C2"/>
+    <mergeCell ref="A5:A13"/>
+    <mergeCell ref="C3:H3"/>
+    <mergeCell ref="I3:N3"/>
+    <mergeCell ref="AD3:AI3"/>
+    <mergeCell ref="V1:X2"/>
     <mergeCell ref="AJ3:AO3"/>
     <mergeCell ref="V5:V13"/>
     <mergeCell ref="A25:A33"/>
@@ -3534,12 +3921,6 @@
     <mergeCell ref="V25:V33"/>
     <mergeCell ref="V35:V43"/>
     <mergeCell ref="X3:AC3"/>
-    <mergeCell ref="A1:C2"/>
-    <mergeCell ref="A5:A13"/>
-    <mergeCell ref="C3:H3"/>
-    <mergeCell ref="I3:N3"/>
-    <mergeCell ref="AD3:AI3"/>
-    <mergeCell ref="V1:X2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>